<commit_message>
added crosscheck for 2010 and warm up for data generation 2021/2010
</commit_message>
<xml_diff>
--- a/crosscheck.xlsx
+++ b/crosscheck.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25928"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="5" documentId="11_A13F24EDC38D6F52D9D0D401147852EA64D46792" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{358E75DF-A2CF-491B-86C7-3564669004BE}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-118" yWindow="-118" windowWidth="20736" windowHeight="11756"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -15,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="82">
   <si>
     <t>Variable</t>
   </si>
@@ -258,12 +257,15 @@
   </si>
   <si>
     <t>P7500S3A1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">X </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -366,7 +368,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -410,14 +412,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -437,7 +442,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -512,23 +517,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -564,23 +552,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -756,23 +727,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:G36"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:H36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="9.7109375" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.6640625" customWidth="1"/>
+    <col min="3" max="3" width="14.88671875" style="1" customWidth="1"/>
     <col min="4" max="4" width="15" style="2" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" customWidth="1"/>
-    <col min="6" max="7" width="8.85546875" style="4"/>
+    <col min="5" max="5" width="11.33203125" customWidth="1"/>
+    <col min="6" max="7" width="8.88671875" style="4"/>
+    <col min="8" max="8" width="8.88671875" style="20"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" s="3" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:8" s="3" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="13" t="s">
         <v>60</v>
       </c>
@@ -791,8 +763,11 @@
       <c r="G2" s="10">
         <v>2007</v>
       </c>
-    </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H2" s="10">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B3" s="15" t="s">
         <v>61</v>
       </c>
@@ -811,8 +786,11 @@
       <c r="G3" s="11" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H3" s="10" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B4" s="15"/>
       <c r="C4" s="7" t="s">
         <v>35</v>
@@ -829,8 +807,11 @@
       <c r="G4" s="11" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H4" s="10" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B5" s="15"/>
       <c r="C5" s="7" t="s">
         <v>37</v>
@@ -847,8 +828,11 @@
       <c r="G5" s="11" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H5" s="10" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B6" s="15"/>
       <c r="C6" s="7" t="s">
         <v>38</v>
@@ -865,8 +849,11 @@
       <c r="G6" s="11" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H6" s="10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B7" s="15"/>
       <c r="C7" s="16" t="s">
         <v>36</v>
@@ -883,12 +870,15 @@
       <c r="G7" s="11" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H7" s="10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B8" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="C8" s="18"/>
+      <c r="C8" s="17"/>
       <c r="D8" s="8" t="s">
         <v>11</v>
       </c>
@@ -901,8 +891,11 @@
       <c r="G8" s="11" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="9" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H8" s="10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" ht="30.15" x14ac:dyDescent="0.3">
       <c r="B9" s="15"/>
       <c r="C9" s="19" t="s">
         <v>34</v>
@@ -919,8 +912,11 @@
       <c r="G9" s="11" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="10" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H9" s="10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B10" s="15"/>
       <c r="C10" s="19"/>
       <c r="D10" s="14" t="s">
@@ -935,8 +931,11 @@
       <c r="G10" s="11" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="11" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H10" s="10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B11" s="15"/>
       <c r="C11" s="19"/>
       <c r="D11" s="14" t="s">
@@ -951,8 +950,11 @@
       <c r="G11" s="11" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H11" s="10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B12" s="15"/>
       <c r="C12" s="16" t="s">
         <v>75</v>
@@ -969,10 +971,13 @@
       <c r="G12" s="11" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H12" s="10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B13" s="15"/>
-      <c r="C13" s="17"/>
+      <c r="C13" s="18"/>
       <c r="D13" s="14" t="s">
         <v>24</v>
       </c>
@@ -985,10 +990,13 @@
       <c r="G13" s="11" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="14" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H13" s="10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" ht="30.15" x14ac:dyDescent="0.3">
       <c r="B14" s="15"/>
-      <c r="C14" s="17"/>
+      <c r="C14" s="18"/>
       <c r="D14" s="14" t="s">
         <v>26</v>
       </c>
@@ -1001,10 +1009,13 @@
       <c r="G14" s="11" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="15" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H14" s="10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" ht="30.15" x14ac:dyDescent="0.3">
       <c r="B15" s="15"/>
-      <c r="C15" s="17"/>
+      <c r="C15" s="18"/>
       <c r="D15" s="14" t="s">
         <v>27</v>
       </c>
@@ -1017,10 +1028,13 @@
       <c r="G15" s="11" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="16" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H15" s="10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B16" s="15"/>
-      <c r="C16" s="18"/>
+      <c r="C16" s="17"/>
       <c r="D16" s="14" t="s">
         <v>28</v>
       </c>
@@ -1031,8 +1045,11 @@
         <v>4</v>
       </c>
       <c r="G16" s="11"/>
-    </row>
-    <row r="17" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H16" s="10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B17" s="15"/>
       <c r="C17" s="12" t="s">
         <v>39</v>
@@ -1049,8 +1066,11 @@
       <c r="G17" s="11" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="18" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H17" s="10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" ht="30.15" x14ac:dyDescent="0.3">
       <c r="B18" s="15"/>
       <c r="C18" s="16" t="s">
         <v>42</v>
@@ -1067,10 +1087,13 @@
       <c r="G18" s="11" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="19" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H18" s="10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" ht="30.15" x14ac:dyDescent="0.3">
       <c r="B19" s="15"/>
-      <c r="C19" s="18"/>
+      <c r="C19" s="17"/>
       <c r="D19" s="8" t="s">
         <v>46</v>
       </c>
@@ -1083,8 +1106,11 @@
       <c r="G19" s="11" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="20" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H19" s="10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" ht="30.15" x14ac:dyDescent="0.3">
       <c r="B20" s="15"/>
       <c r="C20" s="7" t="s">
         <v>47</v>
@@ -1101,8 +1127,11 @@
       <c r="G20" s="11" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="21" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H20" s="10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" ht="30.15" x14ac:dyDescent="0.3">
       <c r="B21" s="15"/>
       <c r="C21" s="7" t="s">
         <v>48</v>
@@ -1119,8 +1148,11 @@
       <c r="G21" s="11" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="22" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H21" s="10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" ht="30.15" x14ac:dyDescent="0.3">
       <c r="B22" s="15"/>
       <c r="C22" s="7" t="s">
         <v>53</v>
@@ -1137,8 +1169,11 @@
       <c r="G22" s="11" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="23" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H22" s="10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" ht="30.15" x14ac:dyDescent="0.3">
       <c r="B23" s="15"/>
       <c r="C23" s="7" t="s">
         <v>56</v>
@@ -1155,8 +1190,11 @@
       <c r="G23" s="11" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="24" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H23" s="10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" ht="30.15" x14ac:dyDescent="0.3">
       <c r="B24" s="7" t="s">
         <v>73</v>
       </c>
@@ -1175,8 +1213,11 @@
       <c r="G24" s="11" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="25" spans="2:7" ht="45.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H24" s="10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" ht="45.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="15" t="s">
         <v>74</v>
       </c>
@@ -1195,10 +1236,13 @@
       <c r="G25" s="11" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="26" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H25" s="10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" ht="15.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="15"/>
-      <c r="C26" s="17"/>
+      <c r="C26" s="18"/>
       <c r="D26" s="8" t="s">
         <v>65</v>
       </c>
@@ -1211,10 +1255,13 @@
       <c r="G26" s="11" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H26" s="10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B27" s="15"/>
-      <c r="C27" s="17"/>
+      <c r="C27" s="18"/>
       <c r="D27" s="8" t="s">
         <v>66</v>
       </c>
@@ -1227,10 +1274,13 @@
       <c r="G27" s="11" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H27" s="10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B28" s="15"/>
-      <c r="C28" s="17"/>
+      <c r="C28" s="18"/>
       <c r="D28" s="8" t="s">
         <v>67</v>
       </c>
@@ -1243,10 +1293,13 @@
       <c r="G28" s="11" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="29" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H28" s="10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B29" s="15"/>
-      <c r="C29" s="18"/>
+      <c r="C29" s="17"/>
       <c r="D29" s="8" t="s">
         <v>68</v>
       </c>
@@ -1259,8 +1312,11 @@
       <c r="G29" s="11" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H29" s="10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B30" s="9"/>
       <c r="C30" s="7" t="s">
         <v>40</v>
@@ -1269,23 +1325,24 @@
       <c r="E30" s="9"/>
       <c r="F30" s="11"/>
       <c r="G30" s="11"/>
-    </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H30" s="10"/>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C32"/>
     </row>
-    <row r="33" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C33"/>
       <c r="E33" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="34" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C34"/>
     </row>
-    <row r="35" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C35"/>
     </row>
-    <row r="36" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C36"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
more crosscheck and small code modifications
</commit_message>
<xml_diff>
--- a/crosscheck.xlsx
+++ b/crosscheck.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="83">
   <si>
     <t>Variable</t>
   </si>
@@ -260,6 +260,9 @@
   </si>
   <si>
     <t xml:space="preserve">X </t>
+  </si>
+  <si>
+    <t>OK SCRIPT</t>
   </si>
 </sst>
 </file>
@@ -368,7 +371,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -409,6 +412,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -420,9 +429,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -728,10 +734,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:H36"/>
+  <dimension ref="B2:J36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+    <sheetView tabSelected="1" topLeftCell="B19" workbookViewId="0">
+      <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
@@ -741,10 +747,11 @@
     <col min="4" max="4" width="15" style="2" customWidth="1"/>
     <col min="5" max="5" width="11.33203125" customWidth="1"/>
     <col min="6" max="7" width="8.88671875" style="4"/>
-    <col min="8" max="8" width="8.88671875" style="20"/>
+    <col min="8" max="8" width="8.88671875" style="16"/>
+    <col min="9" max="9" width="10.77734375" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" s="3" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:10" s="3" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="13" t="s">
         <v>60</v>
       </c>
@@ -766,9 +773,13 @@
       <c r="H2" s="10">
         <v>2010</v>
       </c>
-    </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B3" s="15" t="s">
+      <c r="I2" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="J2"/>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B3" s="17" t="s">
         <v>61</v>
       </c>
       <c r="C3" s="7" t="s">
@@ -789,9 +800,12 @@
       <c r="H3" s="10" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B4" s="15"/>
+      <c r="I3" s="15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B4" s="17"/>
       <c r="C4" s="7" t="s">
         <v>35</v>
       </c>
@@ -810,9 +824,12 @@
       <c r="H4" s="10" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B5" s="15"/>
+      <c r="I4" s="15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B5" s="17"/>
       <c r="C5" s="7" t="s">
         <v>37</v>
       </c>
@@ -831,9 +848,12 @@
       <c r="H5" s="10" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B6" s="15"/>
+      <c r="I5" s="15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B6" s="17"/>
       <c r="C6" s="7" t="s">
         <v>38</v>
       </c>
@@ -852,10 +872,13 @@
       <c r="H6" s="10" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B7" s="15"/>
-      <c r="C7" s="16" t="s">
+      <c r="I6" s="15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B7" s="17"/>
+      <c r="C7" s="18" t="s">
         <v>36</v>
       </c>
       <c r="D7" s="8" t="s">
@@ -873,12 +896,15 @@
       <c r="H7" s="10" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B8" s="15" t="s">
+      <c r="I7" s="15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B8" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="C8" s="17"/>
+      <c r="C8" s="19"/>
       <c r="D8" s="8" t="s">
         <v>11</v>
       </c>
@@ -894,10 +920,13 @@
       <c r="H8" s="10" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="9" spans="2:8" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="B9" s="15"/>
-      <c r="C9" s="19" t="s">
+      <c r="I8" s="15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" ht="30.15" x14ac:dyDescent="0.3">
+      <c r="B9" s="17"/>
+      <c r="C9" s="21" t="s">
         <v>34</v>
       </c>
       <c r="D9" s="14" t="s">
@@ -915,10 +944,13 @@
       <c r="H9" s="10" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B10" s="15"/>
-      <c r="C10" s="19"/>
+      <c r="I9" s="15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B10" s="17"/>
+      <c r="C10" s="21"/>
       <c r="D10" s="14" t="s">
         <v>14</v>
       </c>
@@ -934,10 +966,13 @@
       <c r="H10" s="10" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B11" s="15"/>
-      <c r="C11" s="19"/>
+      <c r="I10" s="15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B11" s="17"/>
+      <c r="C11" s="21"/>
       <c r="D11" s="14" t="s">
         <v>15</v>
       </c>
@@ -953,10 +988,13 @@
       <c r="H11" s="10" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B12" s="15"/>
-      <c r="C12" s="16" t="s">
+      <c r="I11" s="15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B12" s="17"/>
+      <c r="C12" s="18" t="s">
         <v>75</v>
       </c>
       <c r="D12" s="14" t="s">
@@ -974,10 +1012,13 @@
       <c r="H12" s="10" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B13" s="15"/>
-      <c r="C13" s="18"/>
+      <c r="I12" s="15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B13" s="17"/>
+      <c r="C13" s="20"/>
       <c r="D13" s="14" t="s">
         <v>24</v>
       </c>
@@ -993,10 +1034,13 @@
       <c r="H13" s="10" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="14" spans="2:8" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="B14" s="15"/>
-      <c r="C14" s="18"/>
+      <c r="I13" s="15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" ht="30.15" x14ac:dyDescent="0.3">
+      <c r="B14" s="17"/>
+      <c r="C14" s="20"/>
       <c r="D14" s="14" t="s">
         <v>26</v>
       </c>
@@ -1012,10 +1056,13 @@
       <c r="H14" s="10" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="15" spans="2:8" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="B15" s="15"/>
-      <c r="C15" s="18"/>
+      <c r="I14" s="15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" ht="30.15" x14ac:dyDescent="0.3">
+      <c r="B15" s="17"/>
+      <c r="C15" s="20"/>
       <c r="D15" s="14" t="s">
         <v>27</v>
       </c>
@@ -1031,10 +1078,13 @@
       <c r="H15" s="10" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B16" s="15"/>
-      <c r="C16" s="17"/>
+      <c r="I15" s="15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B16" s="17"/>
+      <c r="C16" s="19"/>
       <c r="D16" s="14" t="s">
         <v>28</v>
       </c>
@@ -1048,9 +1098,12 @@
       <c r="H16" s="10" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B17" s="15"/>
+      <c r="I16" s="15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B17" s="17"/>
       <c r="C17" s="12" t="s">
         <v>39</v>
       </c>
@@ -1069,10 +1122,13 @@
       <c r="H17" s="10" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="18" spans="2:8" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="B18" s="15"/>
-      <c r="C18" s="16" t="s">
+      <c r="I17" s="15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" ht="30.15" x14ac:dyDescent="0.3">
+      <c r="B18" s="17"/>
+      <c r="C18" s="18" t="s">
         <v>42</v>
       </c>
       <c r="D18" s="8" t="s">
@@ -1090,10 +1146,13 @@
       <c r="H18" s="10" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="19" spans="2:8" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="B19" s="15"/>
-      <c r="C19" s="17"/>
+      <c r="I18" s="15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" ht="30.15" x14ac:dyDescent="0.3">
+      <c r="B19" s="17"/>
+      <c r="C19" s="19"/>
       <c r="D19" s="8" t="s">
         <v>46</v>
       </c>
@@ -1109,9 +1168,12 @@
       <c r="H19" s="10" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="20" spans="2:8" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="B20" s="15"/>
+      <c r="I19" s="15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" ht="30.15" x14ac:dyDescent="0.3">
+      <c r="B20" s="17"/>
       <c r="C20" s="7" t="s">
         <v>47</v>
       </c>
@@ -1130,9 +1192,12 @@
       <c r="H20" s="10" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="21" spans="2:8" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="B21" s="15"/>
+      <c r="I20" s="15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" ht="30.15" x14ac:dyDescent="0.3">
+      <c r="B21" s="17"/>
       <c r="C21" s="7" t="s">
         <v>48</v>
       </c>
@@ -1151,9 +1216,12 @@
       <c r="H21" s="10" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="22" spans="2:8" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="B22" s="15"/>
+      <c r="I21" s="15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" ht="30.15" x14ac:dyDescent="0.3">
+      <c r="B22" s="17"/>
       <c r="C22" s="7" t="s">
         <v>53</v>
       </c>
@@ -1172,9 +1240,12 @@
       <c r="H22" s="10" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="23" spans="2:8" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="B23" s="15"/>
+      <c r="I22" s="15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" ht="30.15" x14ac:dyDescent="0.3">
+      <c r="B23" s="17"/>
       <c r="C23" s="7" t="s">
         <v>56</v>
       </c>
@@ -1193,8 +1264,11 @@
       <c r="H23" s="10" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="24" spans="2:8" ht="30.15" x14ac:dyDescent="0.3">
+      <c r="I23" s="15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" ht="30.15" x14ac:dyDescent="0.3">
       <c r="B24" s="7" t="s">
         <v>73</v>
       </c>
@@ -1216,12 +1290,15 @@
       <c r="H24" s="10" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="25" spans="2:8" ht="45.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="15" t="s">
+      <c r="I24" s="15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" ht="45.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="C25" s="16" t="s">
+      <c r="C25" s="18" t="s">
         <v>76</v>
       </c>
       <c r="D25" s="8" t="s">
@@ -1239,10 +1316,13 @@
       <c r="H25" s="10" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="26" spans="2:8" ht="15.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="15"/>
-      <c r="C26" s="18"/>
+      <c r="I25" s="15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" ht="15.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="17"/>
+      <c r="C26" s="20"/>
       <c r="D26" s="8" t="s">
         <v>65</v>
       </c>
@@ -1258,10 +1338,13 @@
       <c r="H26" s="10" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B27" s="15"/>
-      <c r="C27" s="18"/>
+      <c r="I26" s="15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B27" s="17"/>
+      <c r="C27" s="20"/>
       <c r="D27" s="8" t="s">
         <v>66</v>
       </c>
@@ -1277,10 +1360,13 @@
       <c r="H27" s="10" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B28" s="15"/>
-      <c r="C28" s="18"/>
+      <c r="I27" s="15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B28" s="17"/>
+      <c r="C28" s="20"/>
       <c r="D28" s="8" t="s">
         <v>67</v>
       </c>
@@ -1296,10 +1382,13 @@
       <c r="H28" s="10" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B29" s="15"/>
-      <c r="C29" s="17"/>
+      <c r="I28" s="15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B29" s="17"/>
+      <c r="C29" s="19"/>
       <c r="D29" s="8" t="s">
         <v>68</v>
       </c>
@@ -1315,8 +1404,11 @@
       <c r="H29" s="10" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I29" s="15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B30" s="9"/>
       <c r="C30" s="7" t="s">
         <v>40</v>
@@ -1326,8 +1418,9 @@
       <c r="F30" s="11"/>
       <c r="G30" s="11"/>
       <c r="H30" s="10"/>
-    </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I30" s="15"/>
+    </row>
+    <row r="32" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C32"/>
     </row>
     <row r="33" spans="3:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
streamlined code to generate first 2021
</commit_message>
<xml_diff>
--- a/crosscheck.xlsx
+++ b/crosscheck.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="84">
   <si>
     <t>Variable</t>
   </si>
@@ -263,6 +263,9 @@
   </si>
   <si>
     <t>OK SCRIPT</t>
+  </si>
+  <si>
+    <t>OK GENERADOR</t>
   </si>
 </sst>
 </file>
@@ -371,7 +374,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -413,6 +416,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -736,8 +742,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:J36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B19" workbookViewId="0">
-      <selection activeCell="I29" sqref="I29"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
@@ -749,6 +755,7 @@
     <col min="6" max="7" width="8.88671875" style="4"/>
     <col min="8" max="8" width="8.88671875" style="16"/>
     <col min="9" max="9" width="10.77734375" style="4" customWidth="1"/>
+    <col min="10" max="10" width="13.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:10" s="3" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -776,10 +783,12 @@
       <c r="I2" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="J2"/>
+      <c r="J2" s="17" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="18" t="s">
         <v>61</v>
       </c>
       <c r="C3" s="7" t="s">
@@ -803,9 +812,10 @@
       <c r="I3" s="15" t="s">
         <v>4</v>
       </c>
+      <c r="J3" s="17"/>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B4" s="17"/>
+      <c r="B4" s="18"/>
       <c r="C4" s="7" t="s">
         <v>35</v>
       </c>
@@ -827,9 +837,10 @@
       <c r="I4" s="15" t="s">
         <v>4</v>
       </c>
+      <c r="J4" s="17"/>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B5" s="17"/>
+      <c r="B5" s="18"/>
       <c r="C5" s="7" t="s">
         <v>37</v>
       </c>
@@ -851,9 +862,10 @@
       <c r="I5" s="15" t="s">
         <v>4</v>
       </c>
+      <c r="J5" s="17"/>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B6" s="17"/>
+      <c r="B6" s="18"/>
       <c r="C6" s="7" t="s">
         <v>38</v>
       </c>
@@ -875,10 +887,11 @@
       <c r="I6" s="15" t="s">
         <v>4</v>
       </c>
+      <c r="J6" s="17"/>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B7" s="17"/>
-      <c r="C7" s="18" t="s">
+      <c r="B7" s="18"/>
+      <c r="C7" s="19" t="s">
         <v>36</v>
       </c>
       <c r="D7" s="8" t="s">
@@ -899,12 +912,13 @@
       <c r="I7" s="15" t="s">
         <v>4</v>
       </c>
+      <c r="J7" s="17"/>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="C8" s="19"/>
+      <c r="C8" s="20"/>
       <c r="D8" s="8" t="s">
         <v>11</v>
       </c>
@@ -923,10 +937,13 @@
       <c r="I8" s="15" t="s">
         <v>4</v>
       </c>
+      <c r="J8" s="17" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="9" spans="2:10" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="B9" s="17"/>
-      <c r="C9" s="21" t="s">
+      <c r="B9" s="18"/>
+      <c r="C9" s="22" t="s">
         <v>34</v>
       </c>
       <c r="D9" s="14" t="s">
@@ -947,10 +964,13 @@
       <c r="I9" s="15" t="s">
         <v>4</v>
       </c>
+      <c r="J9" s="17" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B10" s="17"/>
-      <c r="C10" s="21"/>
+      <c r="B10" s="18"/>
+      <c r="C10" s="22"/>
       <c r="D10" s="14" t="s">
         <v>14</v>
       </c>
@@ -969,10 +989,13 @@
       <c r="I10" s="15" t="s">
         <v>4</v>
       </c>
+      <c r="J10" s="17" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B11" s="17"/>
-      <c r="C11" s="21"/>
+      <c r="B11" s="18"/>
+      <c r="C11" s="22"/>
       <c r="D11" s="14" t="s">
         <v>15</v>
       </c>
@@ -991,10 +1014,13 @@
       <c r="I11" s="15" t="s">
         <v>4</v>
       </c>
+      <c r="J11" s="17" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B12" s="17"/>
-      <c r="C12" s="18" t="s">
+      <c r="B12" s="18"/>
+      <c r="C12" s="19" t="s">
         <v>75</v>
       </c>
       <c r="D12" s="14" t="s">
@@ -1015,10 +1041,13 @@
       <c r="I12" s="15" t="s">
         <v>4</v>
       </c>
+      <c r="J12" s="17" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B13" s="17"/>
-      <c r="C13" s="20"/>
+      <c r="B13" s="18"/>
+      <c r="C13" s="21"/>
       <c r="D13" s="14" t="s">
         <v>24</v>
       </c>
@@ -1037,10 +1066,13 @@
       <c r="I13" s="15" t="s">
         <v>4</v>
       </c>
+      <c r="J13" s="17" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="14" spans="2:10" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="B14" s="17"/>
-      <c r="C14" s="20"/>
+      <c r="B14" s="18"/>
+      <c r="C14" s="21"/>
       <c r="D14" s="14" t="s">
         <v>26</v>
       </c>
@@ -1059,10 +1091,13 @@
       <c r="I14" s="15" t="s">
         <v>4</v>
       </c>
+      <c r="J14" s="17" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="15" spans="2:10" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="B15" s="17"/>
-      <c r="C15" s="20"/>
+      <c r="B15" s="18"/>
+      <c r="C15" s="21"/>
       <c r="D15" s="14" t="s">
         <v>27</v>
       </c>
@@ -1081,10 +1116,13 @@
       <c r="I15" s="15" t="s">
         <v>4</v>
       </c>
+      <c r="J15" s="17" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B16" s="17"/>
-      <c r="C16" s="19"/>
+      <c r="B16" s="18"/>
+      <c r="C16" s="20"/>
       <c r="D16" s="14" t="s">
         <v>28</v>
       </c>
@@ -1101,9 +1139,12 @@
       <c r="I16" s="15" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B17" s="17"/>
+      <c r="J16" s="17" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B17" s="18"/>
       <c r="C17" s="12" t="s">
         <v>39</v>
       </c>
@@ -1125,10 +1166,13 @@
       <c r="I17" s="15" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="18" spans="2:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="B18" s="17"/>
-      <c r="C18" s="18" t="s">
+      <c r="J17" s="17" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" ht="30.15" x14ac:dyDescent="0.3">
+      <c r="B18" s="18"/>
+      <c r="C18" s="19" t="s">
         <v>42</v>
       </c>
       <c r="D18" s="8" t="s">
@@ -1149,10 +1193,13 @@
       <c r="I18" s="15" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="19" spans="2:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="B19" s="17"/>
-      <c r="C19" s="19"/>
+      <c r="J18" s="17" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" ht="30.15" x14ac:dyDescent="0.3">
+      <c r="B19" s="18"/>
+      <c r="C19" s="20"/>
       <c r="D19" s="8" t="s">
         <v>46</v>
       </c>
@@ -1171,9 +1218,12 @@
       <c r="I19" s="15" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="20" spans="2:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="B20" s="17"/>
+      <c r="J19" s="17" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10" ht="30.15" x14ac:dyDescent="0.3">
+      <c r="B20" s="18"/>
       <c r="C20" s="7" t="s">
         <v>47</v>
       </c>
@@ -1195,9 +1245,12 @@
       <c r="I20" s="15" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="21" spans="2:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="B21" s="17"/>
+      <c r="J20" s="17" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10" ht="30.15" x14ac:dyDescent="0.3">
+      <c r="B21" s="18"/>
       <c r="C21" s="7" t="s">
         <v>48</v>
       </c>
@@ -1219,9 +1272,12 @@
       <c r="I21" s="15" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="22" spans="2:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="B22" s="17"/>
+      <c r="J21" s="17" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10" ht="30.15" x14ac:dyDescent="0.3">
+      <c r="B22" s="18"/>
       <c r="C22" s="7" t="s">
         <v>53</v>
       </c>
@@ -1243,9 +1299,12 @@
       <c r="I22" s="15" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="23" spans="2:9" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="B23" s="17"/>
+      <c r="J22" s="17" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="2:10" ht="30.15" x14ac:dyDescent="0.3">
+      <c r="B23" s="18"/>
       <c r="C23" s="7" t="s">
         <v>56</v>
       </c>
@@ -1267,8 +1326,11 @@
       <c r="I23" s="15" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="24" spans="2:9" ht="30.15" x14ac:dyDescent="0.3">
+      <c r="J23" s="17" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="2:10" ht="30.15" x14ac:dyDescent="0.3">
       <c r="B24" s="7" t="s">
         <v>73</v>
       </c>
@@ -1293,12 +1355,13 @@
       <c r="I24" s="15" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="25" spans="2:9" ht="45.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="17" t="s">
+      <c r="J24" s="17"/>
+    </row>
+    <row r="25" spans="2:10" ht="45.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="C25" s="18" t="s">
+      <c r="C25" s="19" t="s">
         <v>76</v>
       </c>
       <c r="D25" s="8" t="s">
@@ -1319,10 +1382,11 @@
       <c r="I25" s="15" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="26" spans="2:9" ht="15.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="17"/>
-      <c r="C26" s="20"/>
+      <c r="J25" s="17"/>
+    </row>
+    <row r="26" spans="2:10" ht="15.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="18"/>
+      <c r="C26" s="21"/>
       <c r="D26" s="8" t="s">
         <v>65</v>
       </c>
@@ -1341,10 +1405,11 @@
       <c r="I26" s="15" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B27" s="17"/>
-      <c r="C27" s="20"/>
+      <c r="J26" s="17"/>
+    </row>
+    <row r="27" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B27" s="18"/>
+      <c r="C27" s="21"/>
       <c r="D27" s="8" t="s">
         <v>66</v>
       </c>
@@ -1363,10 +1428,11 @@
       <c r="I27" s="15" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B28" s="17"/>
-      <c r="C28" s="20"/>
+      <c r="J27" s="17"/>
+    </row>
+    <row r="28" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B28" s="18"/>
+      <c r="C28" s="21"/>
       <c r="D28" s="8" t="s">
         <v>67</v>
       </c>
@@ -1385,10 +1451,11 @@
       <c r="I28" s="15" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B29" s="17"/>
-      <c r="C29" s="19"/>
+      <c r="J28" s="17"/>
+    </row>
+    <row r="29" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B29" s="18"/>
+      <c r="C29" s="20"/>
       <c r="D29" s="8" t="s">
         <v>68</v>
       </c>
@@ -1407,8 +1474,9 @@
       <c r="I29" s="15" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J29" s="17"/>
+    </row>
+    <row r="30" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B30" s="9"/>
       <c r="C30" s="7" t="s">
         <v>40</v>
@@ -1419,8 +1487,9 @@
       <c r="G30" s="11"/>
       <c r="H30" s="10"/>
       <c r="I30" s="15"/>
-    </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J30" s="17"/>
+    </row>
+    <row r="32" spans="2:10" x14ac:dyDescent="0.3">
       <c r="C32"/>
     </row>
     <row r="33" spans="3:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
added all scripts for all file types
</commit_message>
<xml_diff>
--- a/crosscheck.xlsx
+++ b/crosscheck.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="84">
   <si>
     <t>Variable</t>
   </si>
@@ -259,13 +259,13 @@
     <t>P7500S3A1</t>
   </si>
   <si>
-    <t xml:space="preserve">X </t>
-  </si>
-  <si>
     <t>OK SCRIPT</t>
   </si>
   <si>
     <t>OK GENERADOR</t>
+  </si>
+  <si>
+    <t>Nota: 2012 tiene ya los 24 deptos</t>
   </si>
 </sst>
 </file>
@@ -289,12 +289,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="6">
@@ -374,7 +380,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -435,6 +441,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -742,8 +751,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:J36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+    <sheetView tabSelected="1" topLeftCell="C10" workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
@@ -778,13 +787,13 @@
         <v>2007</v>
       </c>
       <c r="H2" s="10">
-        <v>2010</v>
+        <v>2012</v>
       </c>
       <c r="I2" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="J2" s="17" t="s">
         <v>82</v>
-      </c>
-      <c r="J2" s="17" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.3">
@@ -806,9 +815,7 @@
       <c r="G3" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="10" t="s">
-        <v>81</v>
-      </c>
+      <c r="H3" s="10"/>
       <c r="I3" s="15" t="s">
         <v>4</v>
       </c>
@@ -831,9 +838,7 @@
       <c r="G4" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="10" t="s">
-        <v>81</v>
-      </c>
+      <c r="H4" s="10"/>
       <c r="I4" s="15" t="s">
         <v>4</v>
       </c>
@@ -856,9 +861,7 @@
       <c r="G5" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="H5" s="10" t="s">
-        <v>81</v>
-      </c>
+      <c r="H5" s="10"/>
       <c r="I5" s="15" t="s">
         <v>4</v>
       </c>
@@ -881,9 +884,7 @@
       <c r="G6" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="H6" s="10" t="s">
-        <v>4</v>
-      </c>
+      <c r="H6" s="10"/>
       <c r="I6" s="15" t="s">
         <v>4</v>
       </c>
@@ -906,9 +907,7 @@
       <c r="G7" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="H7" s="10" t="s">
-        <v>4</v>
-      </c>
+      <c r="H7" s="10"/>
       <c r="I7" s="15" t="s">
         <v>4</v>
       </c>
@@ -931,13 +930,11 @@
       <c r="G8" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="H8" s="10" t="s">
-        <v>4</v>
-      </c>
+      <c r="H8" s="10"/>
       <c r="I8" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="J8" s="17" t="s">
+      <c r="J8" s="23" t="s">
         <v>4</v>
       </c>
     </row>
@@ -958,13 +955,11 @@
       <c r="G9" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="H9" s="10" t="s">
-        <v>4</v>
-      </c>
+      <c r="H9" s="10"/>
       <c r="I9" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="J9" s="17" t="s">
+      <c r="J9" s="23" t="s">
         <v>4</v>
       </c>
     </row>
@@ -983,13 +978,11 @@
       <c r="G10" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="H10" s="10" t="s">
-        <v>4</v>
-      </c>
+      <c r="H10" s="10"/>
       <c r="I10" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="J10" s="17" t="s">
+      <c r="J10" s="23" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1008,13 +1001,11 @@
       <c r="G11" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="H11" s="10" t="s">
-        <v>4</v>
-      </c>
+      <c r="H11" s="10"/>
       <c r="I11" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="J11" s="17" t="s">
+      <c r="J11" s="23" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1035,13 +1026,11 @@
       <c r="G12" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="H12" s="10" t="s">
-        <v>4</v>
-      </c>
+      <c r="H12" s="10"/>
       <c r="I12" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="J12" s="17" t="s">
+      <c r="J12" s="23" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1060,13 +1049,11 @@
       <c r="G13" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="H13" s="10" t="s">
-        <v>4</v>
-      </c>
+      <c r="H13" s="10"/>
       <c r="I13" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="J13" s="17" t="s">
+      <c r="J13" s="23" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1085,13 +1072,11 @@
       <c r="G14" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="H14" s="10" t="s">
-        <v>4</v>
-      </c>
+      <c r="H14" s="10"/>
       <c r="I14" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="J14" s="17" t="s">
+      <c r="J14" s="23" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1110,13 +1095,11 @@
       <c r="G15" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="H15" s="10" t="s">
-        <v>4</v>
-      </c>
+      <c r="H15" s="10"/>
       <c r="I15" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="J15" s="17" t="s">
+      <c r="J15" s="23" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1133,13 +1116,11 @@
         <v>4</v>
       </c>
       <c r="G16" s="11"/>
-      <c r="H16" s="10" t="s">
-        <v>4</v>
-      </c>
+      <c r="H16" s="10"/>
       <c r="I16" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="J16" s="17" t="s">
+      <c r="J16" s="23" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1160,13 +1141,11 @@
       <c r="G17" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="H17" s="10" t="s">
-        <v>4</v>
-      </c>
+      <c r="H17" s="10"/>
       <c r="I17" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="J17" s="17" t="s">
+      <c r="J17" s="23" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1187,13 +1166,11 @@
       <c r="G18" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="H18" s="10" t="s">
-        <v>4</v>
-      </c>
+      <c r="H18" s="10"/>
       <c r="I18" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="J18" s="17" t="s">
+      <c r="J18" s="23" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1212,13 +1189,11 @@
       <c r="G19" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="H19" s="10" t="s">
-        <v>4</v>
-      </c>
+      <c r="H19" s="10"/>
       <c r="I19" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="J19" s="17" t="s">
+      <c r="J19" s="23" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1239,13 +1214,11 @@
       <c r="G20" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="H20" s="10" t="s">
-        <v>4</v>
-      </c>
+      <c r="H20" s="10"/>
       <c r="I20" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="J20" s="17" t="s">
+      <c r="J20" s="23" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1266,13 +1239,11 @@
       <c r="G21" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="H21" s="10" t="s">
-        <v>4</v>
-      </c>
+      <c r="H21" s="10"/>
       <c r="I21" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="J21" s="17" t="s">
+      <c r="J21" s="23" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1293,13 +1264,11 @@
       <c r="G22" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="H22" s="10" t="s">
-        <v>4</v>
-      </c>
+      <c r="H22" s="10"/>
       <c r="I22" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="J22" s="17" t="s">
+      <c r="J22" s="23" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1320,13 +1289,11 @@
       <c r="G23" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="H23" s="10" t="s">
-        <v>4</v>
-      </c>
+      <c r="H23" s="10"/>
       <c r="I23" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="J23" s="17" t="s">
+      <c r="J23" s="23" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1349,9 +1316,7 @@
       <c r="G24" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="H24" s="10" t="s">
-        <v>4</v>
-      </c>
+      <c r="H24" s="10"/>
       <c r="I24" s="15" t="s">
         <v>4</v>
       </c>
@@ -1376,13 +1341,13 @@
       <c r="G25" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="H25" s="10" t="s">
-        <v>4</v>
-      </c>
+      <c r="H25" s="10"/>
       <c r="I25" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="J25" s="17"/>
+      <c r="J25" s="23" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="26" spans="2:10" ht="15.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="18"/>
@@ -1399,13 +1364,13 @@
       <c r="G26" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="H26" s="10" t="s">
-        <v>4</v>
-      </c>
+      <c r="H26" s="10"/>
       <c r="I26" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="J26" s="17"/>
+      <c r="J26" s="23" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B27" s="18"/>
@@ -1422,13 +1387,13 @@
       <c r="G27" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="H27" s="10" t="s">
-        <v>4</v>
-      </c>
+      <c r="H27" s="10"/>
       <c r="I27" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="J27" s="17"/>
+      <c r="J27" s="23" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="28" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B28" s="18"/>
@@ -1445,13 +1410,13 @@
       <c r="G28" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="H28" s="10" t="s">
-        <v>4</v>
-      </c>
+      <c r="H28" s="10"/>
       <c r="I28" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="J28" s="17"/>
+      <c r="J28" s="23" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B29" s="18"/>
@@ -1468,13 +1433,13 @@
       <c r="G29" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="H29" s="10" t="s">
-        <v>4</v>
-      </c>
+      <c r="H29" s="10"/>
       <c r="I29" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="J29" s="17"/>
+      <c r="J29" s="23" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="30" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B30" s="9"/>
@@ -1500,6 +1465,9 @@
     </row>
     <row r="34" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C34"/>
+      <c r="E34" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="35" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C35"/>

</xml_diff>

<commit_message>
added mutates for most of the variables and edited crosscheck to reflect those changes (only 2021 for now)
</commit_message>
<xml_diff>
--- a/crosscheck.xlsx
+++ b/crosscheck.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="91">
   <si>
     <t>Variable</t>
   </si>
@@ -151,12 +151,6 @@
     <t>P6800</t>
   </si>
   <si>
-    <t>P7045</t>
-  </si>
-  <si>
-    <t>Horas trabajo secundario</t>
-  </si>
-  <si>
     <t>11. Subempleo horas</t>
   </si>
   <si>
@@ -253,9 +247,6 @@
     <t>Nota: 2007 usa otro CIIU y codifica algunas variables distinto</t>
   </si>
   <si>
-    <t>x</t>
-  </si>
-  <si>
     <t>P7500S3A1</t>
   </si>
   <si>
@@ -269,6 +260,33 @@
   </si>
   <si>
     <t>OK GENERADOR 12</t>
+  </si>
+  <si>
+    <t>Ingreso arriendos</t>
+  </si>
+  <si>
+    <t>P7500S1A1</t>
+  </si>
+  <si>
+    <t>P7510S5A1</t>
+  </si>
+  <si>
+    <t>Dividendos</t>
+  </si>
+  <si>
+    <t>Intereses cesantias</t>
+  </si>
+  <si>
+    <t>P7510S6A1</t>
+  </si>
+  <si>
+    <t>Otros tipos</t>
+  </si>
+  <si>
+    <t>P7510S7A1</t>
+  </si>
+  <si>
+    <t>USO INGLABO</t>
   </si>
 </sst>
 </file>
@@ -383,7 +401,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -430,6 +448,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -442,7 +466,38 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -749,10 +804,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:K36"/>
+  <dimension ref="B2:J44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="P9" sqref="P9"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="I38" sqref="I38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
@@ -761,15 +816,16 @@
     <col min="3" max="3" width="14.88671875" style="1" customWidth="1"/>
     <col min="4" max="4" width="15" style="2" customWidth="1"/>
     <col min="5" max="5" width="11.33203125" customWidth="1"/>
-    <col min="6" max="7" width="8.88671875" style="4"/>
-    <col min="8" max="8" width="8.88671875" style="16"/>
-    <col min="9" max="9" width="10.77734375" style="4" customWidth="1"/>
-    <col min="10" max="11" width="18.33203125" customWidth="1"/>
+    <col min="6" max="6" width="8.88671875" style="4"/>
+    <col min="7" max="7" width="8.88671875" style="16"/>
+    <col min="8" max="8" width="10.77734375" style="4" customWidth="1"/>
+    <col min="9" max="9" width="18.33203125" style="3" customWidth="1"/>
+    <col min="10" max="10" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" s="3" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:10" s="3" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="13" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>33</v>
@@ -784,27 +840,24 @@
         <v>2021</v>
       </c>
       <c r="G2" s="10">
-        <v>2007</v>
-      </c>
-      <c r="H2" s="10">
         <v>2012</v>
       </c>
+      <c r="H2" s="10" t="s">
+        <v>78</v>
+      </c>
       <c r="I2" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="J2" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="J2" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="K2" s="10" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B3" s="17" t="s">
-        <v>61</v>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B3" s="19" t="s">
+        <v>59</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>2</v>
@@ -815,18 +868,15 @@
       <c r="F3" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="H3" s="10"/>
-      <c r="I3" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="J3" s="22"/>
-      <c r="K3" s="22"/>
-    </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B4" s="17"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="I3" s="29"/>
+      <c r="J3" s="18"/>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B4" s="19"/>
       <c r="C4" s="7" t="s">
         <v>35</v>
       </c>
@@ -839,18 +889,17 @@
       <c r="F4" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="H4" s="10"/>
-      <c r="I4" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="J4" s="22"/>
-      <c r="K4" s="22"/>
-    </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B5" s="17"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="I4" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="J4" s="18"/>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B5" s="19"/>
       <c r="C5" s="7" t="s">
         <v>37</v>
       </c>
@@ -863,18 +912,17 @@
       <c r="F5" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="H5" s="10"/>
-      <c r="I5" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="J5" s="22"/>
-      <c r="K5" s="22"/>
-    </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B6" s="17"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="I5" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="J5" s="18"/>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B6" s="19"/>
       <c r="C6" s="7" t="s">
         <v>38</v>
       </c>
@@ -887,19 +935,18 @@
       <c r="F6" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="G6" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="H6" s="10"/>
-      <c r="I6" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="J6" s="22"/>
-      <c r="K6" s="22"/>
-    </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B7" s="17"/>
-      <c r="C7" s="18" t="s">
+      <c r="G6" s="10"/>
+      <c r="H6" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="I6" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="J6" s="18"/>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B7" s="19"/>
+      <c r="C7" s="20" t="s">
         <v>36</v>
       </c>
       <c r="D7" s="8" t="s">
@@ -911,21 +958,18 @@
       <c r="F7" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="G7" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="H7" s="10"/>
-      <c r="I7" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="J7" s="22"/>
-      <c r="K7" s="22"/>
-    </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B8" s="17" t="s">
-        <v>62</v>
-      </c>
-      <c r="C8" s="19"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="I7" s="29"/>
+      <c r="J7" s="18"/>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B8" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="C8" s="21"/>
       <c r="D8" s="8" t="s">
         <v>11</v>
       </c>
@@ -935,19 +979,16 @@
       <c r="F8" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="G8" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="H8" s="10"/>
-      <c r="I8" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="J8" s="22"/>
-      <c r="K8" s="22"/>
-    </row>
-    <row r="9" spans="2:11" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="B9" s="17"/>
-      <c r="C9" s="21" t="s">
+      <c r="G8" s="10"/>
+      <c r="H8" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="I8" s="29"/>
+      <c r="J8" s="18"/>
+    </row>
+    <row r="9" spans="2:10" ht="30.15" x14ac:dyDescent="0.3">
+      <c r="B9" s="27"/>
+      <c r="C9" s="23" t="s">
         <v>34</v>
       </c>
       <c r="D9" s="14" t="s">
@@ -959,19 +1000,18 @@
       <c r="F9" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="G9" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="H9" s="10"/>
-      <c r="I9" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="J9" s="22"/>
-      <c r="K9" s="22"/>
-    </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B10" s="17"/>
-      <c r="C10" s="21"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="I9" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="J9" s="18"/>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B10" s="27"/>
+      <c r="C10" s="23"/>
       <c r="D10" s="14" t="s">
         <v>14</v>
       </c>
@@ -981,19 +1021,18 @@
       <c r="F10" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="G10" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="H10" s="10"/>
-      <c r="I10" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="J10" s="22"/>
-      <c r="K10" s="22"/>
-    </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B11" s="17"/>
-      <c r="C11" s="21"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="I10" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="J10" s="18"/>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B11" s="27"/>
+      <c r="C11" s="23"/>
       <c r="D11" s="14" t="s">
         <v>15</v>
       </c>
@@ -1003,20 +1042,19 @@
       <c r="F11" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="G11" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="H11" s="10"/>
-      <c r="I11" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="J11" s="22"/>
-      <c r="K11" s="22"/>
-    </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B12" s="17"/>
-      <c r="C12" s="18" t="s">
-        <v>75</v>
+      <c r="G11" s="10"/>
+      <c r="H11" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="I11" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="J11" s="18"/>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B12" s="27"/>
+      <c r="C12" s="20" t="s">
+        <v>73</v>
       </c>
       <c r="D12" s="14" t="s">
         <v>25</v>
@@ -1027,19 +1065,18 @@
       <c r="F12" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="G12" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="H12" s="10"/>
-      <c r="I12" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="J12" s="22"/>
-      <c r="K12" s="22"/>
-    </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B13" s="17"/>
-      <c r="C13" s="20"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="I12" s="33" t="s">
+        <v>90</v>
+      </c>
+      <c r="J12" s="18"/>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B13" s="27"/>
+      <c r="C13" s="22"/>
       <c r="D13" s="14" t="s">
         <v>24</v>
       </c>
@@ -1049,19 +1086,16 @@
       <c r="F13" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="G13" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="H13" s="10"/>
-      <c r="I13" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="J13" s="22"/>
-      <c r="K13" s="22"/>
-    </row>
-    <row r="14" spans="2:11" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="B14" s="17"/>
-      <c r="C14" s="20"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="I13" s="34"/>
+      <c r="J13" s="18"/>
+    </row>
+    <row r="14" spans="2:10" ht="30.15" x14ac:dyDescent="0.3">
+      <c r="B14" s="27"/>
+      <c r="C14" s="22"/>
       <c r="D14" s="14" t="s">
         <v>26</v>
       </c>
@@ -1071,19 +1105,16 @@
       <c r="F14" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="G14" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="H14" s="10"/>
-      <c r="I14" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="J14" s="22"/>
-      <c r="K14" s="22"/>
-    </row>
-    <row r="15" spans="2:11" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="B15" s="17"/>
-      <c r="C15" s="20"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="I14" s="34"/>
+      <c r="J14" s="18"/>
+    </row>
+    <row r="15" spans="2:10" ht="30.15" x14ac:dyDescent="0.3">
+      <c r="B15" s="27"/>
+      <c r="C15" s="22"/>
       <c r="D15" s="14" t="s">
         <v>27</v>
       </c>
@@ -1093,19 +1124,16 @@
       <c r="F15" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="G15" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="H15" s="10"/>
-      <c r="I15" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="J15" s="22"/>
-      <c r="K15" s="22"/>
-    </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B16" s="17"/>
-      <c r="C16" s="19"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="I15" s="34"/>
+      <c r="J15" s="18"/>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B16" s="27"/>
+      <c r="C16" s="21"/>
       <c r="D16" s="14" t="s">
         <v>28</v>
       </c>
@@ -1115,16 +1143,15 @@
       <c r="F16" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="G16" s="11"/>
-      <c r="H16" s="10"/>
-      <c r="I16" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="J16" s="22"/>
-      <c r="K16" s="22"/>
-    </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B17" s="17"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="I16" s="35"/>
+      <c r="J16" s="18"/>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B17" s="27"/>
       <c r="C17" s="12" t="s">
         <v>39</v>
       </c>
@@ -1137,19 +1164,16 @@
       <c r="F17" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="G17" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="H17" s="10"/>
-      <c r="I17" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="J17" s="22"/>
-      <c r="K17" s="22"/>
-    </row>
-    <row r="18" spans="2:11" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="B18" s="17"/>
-      <c r="C18" s="18" t="s">
+      <c r="G17" s="10"/>
+      <c r="H17" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="I17" s="29"/>
+      <c r="J17" s="18"/>
+    </row>
+    <row r="18" spans="2:10" ht="30.15" x14ac:dyDescent="0.3">
+      <c r="B18" s="27"/>
+      <c r="C18" s="24" t="s">
         <v>42</v>
       </c>
       <c r="D18" s="8" t="s">
@@ -1161,319 +1185,363 @@
       <c r="F18" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="G18" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="H18" s="10"/>
-      <c r="I18" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="J18" s="22"/>
-      <c r="K18" s="22"/>
-    </row>
-    <row r="19" spans="2:11" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="B19" s="17"/>
-      <c r="C19" s="19"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="I18" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="J18" s="18"/>
+    </row>
+    <row r="19" spans="2:10" ht="30.15" x14ac:dyDescent="0.3">
+      <c r="B19" s="27"/>
+      <c r="C19" s="7" t="s">
+        <v>45</v>
+      </c>
       <c r="D19" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="F19" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="G19" s="10"/>
+      <c r="H19" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="I19" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="J19" s="18"/>
+    </row>
+    <row r="20" spans="2:10" ht="30.15" x14ac:dyDescent="0.3">
+      <c r="B20" s="27"/>
+      <c r="C20" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="E19" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="F19" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="G19" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="H19" s="10"/>
-      <c r="I19" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="J19" s="22"/>
-      <c r="K19" s="22"/>
-    </row>
-    <row r="20" spans="2:11" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="B20" s="17"/>
-      <c r="C20" s="7" t="s">
-        <v>47</v>
-      </c>
       <c r="D20" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="E20" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="E20" s="9" t="s">
-        <v>50</v>
-      </c>
       <c r="F20" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="G20" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="H20" s="10"/>
-      <c r="I20" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="J20" s="22"/>
-      <c r="K20" s="22"/>
-    </row>
-    <row r="21" spans="2:11" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="B21" s="17"/>
+      <c r="G20" s="10"/>
+      <c r="H20" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="I20" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="J20" s="18"/>
+    </row>
+    <row r="21" spans="2:10" ht="30.15" x14ac:dyDescent="0.3">
+      <c r="B21" s="27"/>
       <c r="C21" s="7" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="D21" s="8" t="s">
         <v>52</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="F21" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="G21" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="H21" s="10"/>
-      <c r="I21" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="J21" s="22"/>
-      <c r="K21" s="22"/>
-    </row>
-    <row r="22" spans="2:11" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="B22" s="17"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="I21" s="29"/>
+      <c r="J21" s="18"/>
+    </row>
+    <row r="22" spans="2:10" ht="30.15" x14ac:dyDescent="0.3">
+      <c r="B22" s="28"/>
       <c r="C22" s="7" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E22" s="9" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F22" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="G22" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="H22" s="10"/>
-      <c r="I22" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="J22" s="22"/>
-      <c r="K22" s="22"/>
-    </row>
-    <row r="23" spans="2:11" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="B23" s="17"/>
+      <c r="G22" s="10"/>
+      <c r="H22" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="I22" s="29"/>
+      <c r="J22" s="18"/>
+    </row>
+    <row r="23" spans="2:10" ht="30.15" x14ac:dyDescent="0.3">
+      <c r="B23" s="7" t="s">
+        <v>71</v>
+      </c>
       <c r="C23" s="7" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
       <c r="E23" s="9" t="s">
-        <v>58</v>
+        <v>75</v>
       </c>
       <c r="F23" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="G23" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="H23" s="10"/>
-      <c r="I23" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="J23" s="22"/>
-      <c r="K23" s="22"/>
-    </row>
-    <row r="24" spans="2:11" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="B24" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="C24" s="7" t="s">
-        <v>41</v>
+      <c r="G23" s="10"/>
+      <c r="H23" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="I23" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="J23" s="18"/>
+    </row>
+    <row r="24" spans="2:10" ht="45.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="C24" s="23" t="s">
+        <v>74</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="E24" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="E24" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="F24" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="G24" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="H24" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="I24" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="J24" s="9"/>
+    </row>
+    <row r="25" spans="2:10" ht="15.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="19"/>
+      <c r="C25" s="23"/>
+      <c r="D25" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="E25" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="F25" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="G25" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="H25" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="I25" s="31"/>
+      <c r="J25" s="18"/>
+    </row>
+    <row r="26" spans="2:10" ht="30.15" x14ac:dyDescent="0.3">
+      <c r="B26" s="19"/>
+      <c r="C26" s="23"/>
+      <c r="D26" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="E26" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="F24" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="G24" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="H24" s="10"/>
-      <c r="I24" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="J24" s="22"/>
-      <c r="K24" s="22"/>
-    </row>
-    <row r="25" spans="2:11" ht="45.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="17" t="s">
-        <v>74</v>
-      </c>
-      <c r="C25" s="18" t="s">
+      <c r="F26" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="G26" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="H26" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="I26" s="31"/>
+      <c r="J26" s="18"/>
+    </row>
+    <row r="27" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B27" s="19"/>
+      <c r="C27" s="23"/>
+      <c r="D27" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="E27" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="F27" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="G27" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="H27" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="I27" s="31"/>
+      <c r="J27" s="18"/>
+    </row>
+    <row r="28" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B28" s="19"/>
+      <c r="C28" s="23"/>
+      <c r="D28" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="E28" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="F28" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="G28" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="H28" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="I28" s="31"/>
+      <c r="J28" s="18"/>
+    </row>
+    <row r="29" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B29" s="19"/>
+      <c r="C29" s="23"/>
+      <c r="D29" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="E29" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="F29" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="G29" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="H29" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="I29" s="31"/>
+      <c r="J29" s="18"/>
+    </row>
+    <row r="30" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B30" s="19"/>
+      <c r="C30" s="23"/>
+      <c r="D30" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="E30" s="25" t="s">
+        <v>84</v>
+      </c>
+      <c r="F30" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="G30" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="H30" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="I30" s="31"/>
+      <c r="J30" s="9"/>
+    </row>
+    <row r="31" spans="2:10" ht="30.15" x14ac:dyDescent="0.3">
+      <c r="B31" s="19"/>
+      <c r="C31" s="23"/>
+      <c r="D31" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="E31" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="F31" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="G31" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="H31" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="I31" s="31"/>
+      <c r="J31" s="9"/>
+    </row>
+    <row r="32" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B32" s="19"/>
+      <c r="C32" s="23"/>
+      <c r="D32" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="E32" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="F32" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="G32" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="H32" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="I32" s="32"/>
+      <c r="J32" s="9"/>
+    </row>
+    <row r="33" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B33" s="9"/>
+      <c r="C33" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D33" s="8"/>
+      <c r="E33" s="9"/>
+      <c r="F33" s="11"/>
+      <c r="G33" s="10"/>
+      <c r="H33" s="15"/>
+      <c r="I33" s="29"/>
+      <c r="J33" s="18"/>
+    </row>
+    <row r="34" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="C34"/>
+    </row>
+    <row r="35" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="C35"/>
+    </row>
+    <row r="43" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="E43" t="s">
         <v>76</v>
       </c>
-      <c r="D25" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="E25" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="F25" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="G25" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="H25" s="10"/>
-      <c r="I25" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="J25" s="22"/>
-      <c r="K25" s="22"/>
-    </row>
-    <row r="26" spans="2:11" ht="15.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="17"/>
-      <c r="C26" s="20"/>
-      <c r="D26" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="E26" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="F26" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="G26" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="H26" s="10"/>
-      <c r="I26" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="J26" s="22"/>
-      <c r="K26" s="22"/>
-    </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B27" s="17"/>
-      <c r="C27" s="20"/>
-      <c r="D27" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="E27" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="F27" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="G27" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="H27" s="10"/>
-      <c r="I27" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="J27" s="22"/>
-      <c r="K27" s="22"/>
-    </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B28" s="17"/>
-      <c r="C28" s="20"/>
-      <c r="D28" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="E28" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="F28" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="G28" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="H28" s="10"/>
-      <c r="I28" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="J28" s="22"/>
-      <c r="K28" s="22"/>
-    </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B29" s="17"/>
-      <c r="C29" s="19"/>
-      <c r="D29" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="E29" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="F29" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="G29" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="H29" s="10"/>
-      <c r="I29" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="J29" s="22"/>
-      <c r="K29" s="22"/>
-    </row>
-    <row r="30" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B30" s="9"/>
-      <c r="C30" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="D30" s="8"/>
-      <c r="E30" s="9"/>
-      <c r="F30" s="11"/>
-      <c r="G30" s="11"/>
-      <c r="H30" s="10"/>
-      <c r="I30" s="15"/>
-      <c r="J30" s="22"/>
-      <c r="K30" s="22"/>
-    </row>
-    <row r="32" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="C32"/>
-    </row>
-    <row r="33" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C33"/>
-      <c r="E33" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="34" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C34"/>
-      <c r="E34" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="35" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C35"/>
-    </row>
-    <row r="36" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C36"/>
+    </row>
+    <row r="44" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="E44" t="s">
+        <v>79</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="9">
+    <mergeCell ref="B24:B32"/>
+    <mergeCell ref="C24:C32"/>
+    <mergeCell ref="I24:I32"/>
+    <mergeCell ref="I12:I16"/>
+    <mergeCell ref="B8:B22"/>
     <mergeCell ref="B3:B7"/>
     <mergeCell ref="C7:C8"/>
-    <mergeCell ref="B25:B29"/>
-    <mergeCell ref="C25:C29"/>
     <mergeCell ref="C9:C11"/>
     <mergeCell ref="C12:C16"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="B8:B23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
added one more variable in ocup
</commit_message>
<xml_diff>
--- a/crosscheck.xlsx
+++ b/crosscheck.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="91">
   <si>
     <t>Variable</t>
   </si>
@@ -310,7 +310,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -320,6 +320,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -401,7 +413,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -432,9 +444,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -451,7 +460,44 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -463,41 +509,39 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -806,8 +850,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:J44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="I38" sqref="I38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33:I33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
@@ -817,14 +861,14 @@
     <col min="4" max="4" width="15" style="2" customWidth="1"/>
     <col min="5" max="5" width="11.33203125" customWidth="1"/>
     <col min="6" max="6" width="8.88671875" style="4"/>
-    <col min="7" max="7" width="8.88671875" style="16"/>
+    <col min="7" max="7" width="8.88671875" style="15"/>
     <col min="8" max="8" width="10.77734375" style="4" customWidth="1"/>
     <col min="9" max="9" width="18.33203125" style="3" customWidth="1"/>
     <col min="10" max="10" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:10" s="3" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="12" t="s">
         <v>58</v>
       </c>
       <c r="C2" s="5" t="s">
@@ -853,7 +897,7 @@
       </c>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="21" t="s">
         <v>59</v>
       </c>
       <c r="C3" s="7" t="s">
@@ -869,14 +913,14 @@
         <v>4</v>
       </c>
       <c r="G3" s="10"/>
-      <c r="H3" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="I3" s="29"/>
-      <c r="J3" s="18"/>
+      <c r="H3" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="I3" s="20"/>
+      <c r="J3" s="17"/>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B4" s="19"/>
+      <c r="B4" s="21"/>
       <c r="C4" s="7" t="s">
         <v>35</v>
       </c>
@@ -890,16 +934,16 @@
         <v>4</v>
       </c>
       <c r="G4" s="10"/>
-      <c r="H4" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="I4" s="29" t="s">
-        <v>4</v>
-      </c>
-      <c r="J4" s="18"/>
+      <c r="H4" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="I4" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="J4" s="17"/>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B5" s="19"/>
+      <c r="B5" s="21"/>
       <c r="C5" s="7" t="s">
         <v>37</v>
       </c>
@@ -913,16 +957,16 @@
         <v>4</v>
       </c>
       <c r="G5" s="10"/>
-      <c r="H5" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="I5" s="29" t="s">
-        <v>4</v>
-      </c>
-      <c r="J5" s="18"/>
+      <c r="H5" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="I5" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="J5" s="17"/>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B6" s="19"/>
+      <c r="B6" s="21"/>
       <c r="C6" s="7" t="s">
         <v>38</v>
       </c>
@@ -936,62 +980,62 @@
         <v>4</v>
       </c>
       <c r="G6" s="10"/>
-      <c r="H6" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="I6" s="29" t="s">
-        <v>4</v>
-      </c>
-      <c r="J6" s="18"/>
+      <c r="H6" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="I6" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="J6" s="17"/>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B7" s="19"/>
-      <c r="C7" s="20" t="s">
+      <c r="B7" s="21"/>
+      <c r="C7" s="39" t="s">
         <v>36</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="9" t="s">
+      <c r="E7" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="G7" s="10"/>
-      <c r="H7" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="I7" s="29"/>
-      <c r="J7" s="18"/>
+      <c r="F7" s="37" t="s">
+        <v>4</v>
+      </c>
+      <c r="G7" s="38"/>
+      <c r="H7" s="37" t="s">
+        <v>4</v>
+      </c>
+      <c r="I7" s="38"/>
+      <c r="J7" s="17"/>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B8" s="26" t="s">
+      <c r="B8" s="29" t="s">
         <v>60</v>
       </c>
-      <c r="C8" s="21"/>
-      <c r="D8" s="8" t="s">
+      <c r="C8" s="40"/>
+      <c r="D8" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="E8" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="F8" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="G8" s="10"/>
-      <c r="H8" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="I8" s="29"/>
-      <c r="J8" s="18"/>
+      <c r="F8" s="37" t="s">
+        <v>4</v>
+      </c>
+      <c r="G8" s="38"/>
+      <c r="H8" s="37" t="s">
+        <v>4</v>
+      </c>
+      <c r="I8" s="38"/>
+      <c r="J8" s="17"/>
     </row>
     <row r="9" spans="2:10" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="B9" s="27"/>
-      <c r="C9" s="23" t="s">
+      <c r="B9" s="30"/>
+      <c r="C9" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="D9" s="14" t="s">
+      <c r="D9" s="13" t="s">
         <v>13</v>
       </c>
       <c r="E9" s="9" t="s">
@@ -1001,18 +1045,18 @@
         <v>4</v>
       </c>
       <c r="G9" s="10"/>
-      <c r="H9" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="I9" s="29" t="s">
-        <v>4</v>
-      </c>
-      <c r="J9" s="18"/>
+      <c r="H9" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="I9" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="J9" s="17"/>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B10" s="27"/>
-      <c r="C10" s="23"/>
-      <c r="D10" s="14" t="s">
+      <c r="B10" s="30"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="13" t="s">
         <v>14</v>
       </c>
       <c r="E10" s="9" t="s">
@@ -1022,18 +1066,18 @@
         <v>4</v>
       </c>
       <c r="G10" s="10"/>
-      <c r="H10" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="I10" s="29" t="s">
-        <v>4</v>
-      </c>
-      <c r="J10" s="18"/>
+      <c r="H10" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="I10" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="J10" s="17"/>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B11" s="27"/>
-      <c r="C11" s="23"/>
-      <c r="D11" s="14" t="s">
+      <c r="B11" s="30"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="13" t="s">
         <v>15</v>
       </c>
       <c r="E11" s="9" t="s">
@@ -1043,20 +1087,20 @@
         <v>4</v>
       </c>
       <c r="G11" s="10"/>
-      <c r="H11" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="I11" s="29" t="s">
-        <v>4</v>
-      </c>
-      <c r="J11" s="18"/>
+      <c r="H11" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="I11" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="J11" s="17"/>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B12" s="27"/>
-      <c r="C12" s="20" t="s">
+      <c r="B12" s="30"/>
+      <c r="C12" s="32" t="s">
         <v>73</v>
       </c>
-      <c r="D12" s="14" t="s">
+      <c r="D12" s="13" t="s">
         <v>25</v>
       </c>
       <c r="E12" s="9" t="s">
@@ -1066,18 +1110,18 @@
         <v>4</v>
       </c>
       <c r="G12" s="10"/>
-      <c r="H12" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="I12" s="33" t="s">
+      <c r="H12" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="I12" s="26" t="s">
         <v>90</v>
       </c>
-      <c r="J12" s="18"/>
+      <c r="J12" s="17"/>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B13" s="27"/>
-      <c r="C13" s="22"/>
-      <c r="D13" s="14" t="s">
+      <c r="B13" s="30"/>
+      <c r="C13" s="34"/>
+      <c r="D13" s="13" t="s">
         <v>24</v>
       </c>
       <c r="E13" s="9" t="s">
@@ -1087,16 +1131,16 @@
         <v>4</v>
       </c>
       <c r="G13" s="10"/>
-      <c r="H13" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="I13" s="34"/>
-      <c r="J13" s="18"/>
+      <c r="H13" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="I13" s="27"/>
+      <c r="J13" s="17"/>
     </row>
     <row r="14" spans="2:10" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="B14" s="27"/>
-      <c r="C14" s="22"/>
-      <c r="D14" s="14" t="s">
+      <c r="B14" s="30"/>
+      <c r="C14" s="34"/>
+      <c r="D14" s="13" t="s">
         <v>26</v>
       </c>
       <c r="E14" s="9" t="s">
@@ -1106,16 +1150,16 @@
         <v>4</v>
       </c>
       <c r="G14" s="10"/>
-      <c r="H14" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="I14" s="34"/>
-      <c r="J14" s="18"/>
+      <c r="H14" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="I14" s="27"/>
+      <c r="J14" s="17"/>
     </row>
     <row r="15" spans="2:10" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="B15" s="27"/>
-      <c r="C15" s="22"/>
-      <c r="D15" s="14" t="s">
+      <c r="B15" s="30"/>
+      <c r="C15" s="34"/>
+      <c r="D15" s="13" t="s">
         <v>27</v>
       </c>
       <c r="E15" s="9" t="s">
@@ -1125,16 +1169,16 @@
         <v>4</v>
       </c>
       <c r="G15" s="10"/>
-      <c r="H15" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="I15" s="34"/>
-      <c r="J15" s="18"/>
+      <c r="H15" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="I15" s="27"/>
+      <c r="J15" s="17"/>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B16" s="27"/>
-      <c r="C16" s="21"/>
-      <c r="D16" s="14" t="s">
+      <c r="B16" s="30"/>
+      <c r="C16" s="33"/>
+      <c r="D16" s="13" t="s">
         <v>28</v>
       </c>
       <c r="E16" s="9" t="s">
@@ -1144,36 +1188,36 @@
         <v>4</v>
       </c>
       <c r="G16" s="10"/>
-      <c r="H16" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="I16" s="35"/>
-      <c r="J16" s="18"/>
+      <c r="H16" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="I16" s="28"/>
+      <c r="J16" s="17"/>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B17" s="27"/>
-      <c r="C17" s="12" t="s">
+      <c r="B17" s="30"/>
+      <c r="C17" s="41" t="s">
         <v>39</v>
       </c>
-      <c r="D17" s="8" t="s">
+      <c r="D17" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="E17" s="9" t="s">
+      <c r="E17" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="F17" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="G17" s="10"/>
-      <c r="H17" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="I17" s="29"/>
-      <c r="J17" s="18"/>
+      <c r="F17" s="37" t="s">
+        <v>4</v>
+      </c>
+      <c r="G17" s="38"/>
+      <c r="H17" s="37" t="s">
+        <v>4</v>
+      </c>
+      <c r="I17" s="38"/>
+      <c r="J17" s="17"/>
     </row>
     <row r="18" spans="2:10" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="B18" s="27"/>
-      <c r="C18" s="24" t="s">
+      <c r="B18" s="30"/>
+      <c r="C18" s="18" t="s">
         <v>42</v>
       </c>
       <c r="D18" s="8" t="s">
@@ -1186,16 +1230,16 @@
         <v>4</v>
       </c>
       <c r="G18" s="10"/>
-      <c r="H18" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="I18" s="29" t="s">
-        <v>4</v>
-      </c>
-      <c r="J18" s="18"/>
+      <c r="H18" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="I18" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="J18" s="17"/>
     </row>
     <row r="19" spans="2:10" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="B19" s="27"/>
+      <c r="B19" s="30"/>
       <c r="C19" s="7" t="s">
         <v>45</v>
       </c>
@@ -1209,16 +1253,16 @@
         <v>4</v>
       </c>
       <c r="G19" s="10"/>
-      <c r="H19" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="I19" s="29" t="s">
-        <v>4</v>
-      </c>
-      <c r="J19" s="18"/>
+      <c r="H19" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="I19" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="J19" s="17"/>
     </row>
     <row r="20" spans="2:10" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="B20" s="27"/>
+      <c r="B20" s="30"/>
       <c r="C20" s="7" t="s">
         <v>46</v>
       </c>
@@ -1232,16 +1276,16 @@
         <v>4</v>
       </c>
       <c r="G20" s="10"/>
-      <c r="H20" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="I20" s="29" t="s">
-        <v>4</v>
-      </c>
-      <c r="J20" s="18"/>
+      <c r="H20" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="I20" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="J20" s="17"/>
     </row>
     <row r="21" spans="2:10" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="B21" s="27"/>
+      <c r="B21" s="30"/>
       <c r="C21" s="7" t="s">
         <v>51</v>
       </c>
@@ -1255,32 +1299,34 @@
         <v>4</v>
       </c>
       <c r="G21" s="10"/>
-      <c r="H21" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="I21" s="29"/>
-      <c r="J21" s="18"/>
+      <c r="H21" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="I21" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="J21" s="17"/>
     </row>
     <row r="22" spans="2:10" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="B22" s="28"/>
-      <c r="C22" s="7" t="s">
+      <c r="B22" s="31"/>
+      <c r="C22" s="42" t="s">
         <v>54</v>
       </c>
-      <c r="D22" s="8" t="s">
+      <c r="D22" s="35" t="s">
         <v>55</v>
       </c>
-      <c r="E22" s="9" t="s">
+      <c r="E22" s="36" t="s">
         <v>56</v>
       </c>
-      <c r="F22" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="G22" s="10"/>
-      <c r="H22" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="I22" s="29"/>
-      <c r="J22" s="18"/>
+      <c r="F22" s="37" t="s">
+        <v>4</v>
+      </c>
+      <c r="G22" s="38"/>
+      <c r="H22" s="37" t="s">
+        <v>4</v>
+      </c>
+      <c r="I22" s="38"/>
+      <c r="J22" s="17"/>
     </row>
     <row r="23" spans="2:10" ht="30.15" x14ac:dyDescent="0.3">
       <c r="B23" s="7" t="s">
@@ -1299,221 +1345,221 @@
         <v>4</v>
       </c>
       <c r="G23" s="10"/>
-      <c r="H23" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="I23" s="29" t="s">
-        <v>4</v>
-      </c>
-      <c r="J23" s="18"/>
+      <c r="H23" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="I23" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="J23" s="17"/>
     </row>
     <row r="24" spans="2:10" ht="45.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="19" t="s">
+      <c r="B24" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="C24" s="23" t="s">
+      <c r="C24" s="22" t="s">
         <v>74</v>
       </c>
       <c r="D24" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="E24" s="25" t="s">
+      <c r="E24" s="19" t="s">
         <v>83</v>
       </c>
-      <c r="F24" s="17" t="s">
+      <c r="F24" s="16" t="s">
         <v>4</v>
       </c>
       <c r="G24" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="H24" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="I24" s="30" t="s">
+      <c r="H24" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="I24" s="23" t="s">
         <v>4</v>
       </c>
       <c r="J24" s="9"/>
     </row>
     <row r="25" spans="2:10" ht="15.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="19"/>
-      <c r="C25" s="23"/>
+      <c r="B25" s="21"/>
+      <c r="C25" s="22"/>
       <c r="D25" s="8" t="s">
         <v>61</v>
       </c>
       <c r="E25" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="F25" s="17" t="s">
+      <c r="F25" s="16" t="s">
         <v>4</v>
       </c>
       <c r="G25" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="H25" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="I25" s="31"/>
-      <c r="J25" s="18"/>
+      <c r="H25" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="I25" s="24"/>
+      <c r="J25" s="17"/>
     </row>
     <row r="26" spans="2:10" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="B26" s="19"/>
-      <c r="C26" s="23"/>
+      <c r="B26" s="21"/>
+      <c r="C26" s="22"/>
       <c r="D26" s="8" t="s">
         <v>63</v>
       </c>
       <c r="E26" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="F26" s="17" t="s">
+      <c r="F26" s="16" t="s">
         <v>4</v>
       </c>
       <c r="G26" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="H26" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="I26" s="31"/>
-      <c r="J26" s="18"/>
+      <c r="H26" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="I26" s="24"/>
+      <c r="J26" s="17"/>
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B27" s="19"/>
-      <c r="C27" s="23"/>
+      <c r="B27" s="21"/>
+      <c r="C27" s="22"/>
       <c r="D27" s="8" t="s">
         <v>64</v>
       </c>
       <c r="E27" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="F27" s="17" t="s">
+      <c r="F27" s="16" t="s">
         <v>4</v>
       </c>
       <c r="G27" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="H27" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="I27" s="31"/>
-      <c r="J27" s="18"/>
+      <c r="H27" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="I27" s="24"/>
+      <c r="J27" s="17"/>
     </row>
     <row r="28" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B28" s="19"/>
-      <c r="C28" s="23"/>
+      <c r="B28" s="21"/>
+      <c r="C28" s="22"/>
       <c r="D28" s="8" t="s">
         <v>65</v>
       </c>
       <c r="E28" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="F28" s="17" t="s">
+      <c r="F28" s="16" t="s">
         <v>4</v>
       </c>
       <c r="G28" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="H28" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="I28" s="31"/>
-      <c r="J28" s="18"/>
+      <c r="H28" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="I28" s="24"/>
+      <c r="J28" s="17"/>
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B29" s="19"/>
-      <c r="C29" s="23"/>
+      <c r="B29" s="21"/>
+      <c r="C29" s="22"/>
       <c r="D29" s="8" t="s">
         <v>66</v>
       </c>
       <c r="E29" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="F29" s="17" t="s">
+      <c r="F29" s="16" t="s">
         <v>4</v>
       </c>
       <c r="G29" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="H29" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="I29" s="31"/>
-      <c r="J29" s="18"/>
+      <c r="H29" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="I29" s="24"/>
+      <c r="J29" s="17"/>
     </row>
     <row r="30" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B30" s="19"/>
-      <c r="C30" s="23"/>
+      <c r="B30" s="21"/>
+      <c r="C30" s="22"/>
       <c r="D30" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="E30" s="25" t="s">
+      <c r="E30" s="19" t="s">
         <v>84</v>
       </c>
-      <c r="F30" s="17" t="s">
+      <c r="F30" s="16" t="s">
         <v>4</v>
       </c>
       <c r="G30" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="H30" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="I30" s="31"/>
+      <c r="H30" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="I30" s="24"/>
       <c r="J30" s="9"/>
     </row>
     <row r="31" spans="2:10" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="B31" s="19"/>
-      <c r="C31" s="23"/>
+      <c r="B31" s="21"/>
+      <c r="C31" s="22"/>
       <c r="D31" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="E31" s="25" t="s">
+      <c r="E31" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="F31" s="17" t="s">
+      <c r="F31" s="16" t="s">
         <v>4</v>
       </c>
       <c r="G31" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="H31" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="I31" s="31"/>
+      <c r="H31" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="I31" s="24"/>
       <c r="J31" s="9"/>
     </row>
     <row r="32" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B32" s="19"/>
-      <c r="C32" s="23"/>
+      <c r="B32" s="21"/>
+      <c r="C32" s="22"/>
       <c r="D32" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="E32" s="25" t="s">
+      <c r="E32" s="19" t="s">
         <v>89</v>
       </c>
-      <c r="F32" s="17" t="s">
+      <c r="F32" s="16" t="s">
         <v>4</v>
       </c>
       <c r="G32" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="H32" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="I32" s="32"/>
+      <c r="H32" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="I32" s="25"/>
       <c r="J32" s="9"/>
     </row>
     <row r="33" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B33" s="9"/>
-      <c r="C33" s="7" t="s">
+      <c r="C33" s="43" t="s">
         <v>40</v>
       </c>
-      <c r="D33" s="8"/>
-      <c r="E33" s="9"/>
-      <c r="F33" s="11"/>
-      <c r="G33" s="10"/>
-      <c r="H33" s="15"/>
-      <c r="I33" s="29"/>
-      <c r="J33" s="18"/>
+      <c r="D33" s="44"/>
+      <c r="E33" s="45"/>
+      <c r="F33" s="46"/>
+      <c r="G33" s="47"/>
+      <c r="H33" s="46"/>
+      <c r="I33" s="47"/>
+      <c r="J33" s="17"/>
     </row>
     <row r="34" spans="2:10" x14ac:dyDescent="0.3">
       <c r="C34"/>
@@ -1533,15 +1579,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="B3:B7"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="C12:C16"/>
     <mergeCell ref="B24:B32"/>
     <mergeCell ref="C24:C32"/>
     <mergeCell ref="I24:I32"/>
     <mergeCell ref="I12:I16"/>
     <mergeCell ref="B8:B22"/>
-    <mergeCell ref="B3:B7"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="C9:C11"/>
-    <mergeCell ref="C12:C16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
finished all scripts for 2021 excluding SS and hijos
</commit_message>
<xml_diff>
--- a/crosscheck.xlsx
+++ b/crosscheck.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="108">
   <si>
     <t>Variable</t>
   </si>
@@ -287,6 +287,57 @@
   </si>
   <si>
     <t>USO INGLABO</t>
+  </si>
+  <si>
+    <t>VARIABLE DICCIONARIO</t>
+  </si>
+  <si>
+    <t>conformeContrato</t>
+  </si>
+  <si>
+    <t>quiereCambiar</t>
+  </si>
+  <si>
+    <t>conformeTrabajo</t>
+  </si>
+  <si>
+    <t>ingresosTrabajo</t>
+  </si>
+  <si>
+    <t>horasTrabajo</t>
+  </si>
+  <si>
+    <t>subempleadoHoras</t>
+  </si>
+  <si>
+    <t>subempleadoIngresos</t>
+  </si>
+  <si>
+    <t>posicionOcupacional</t>
+  </si>
+  <si>
+    <t>actividadEconomica</t>
+  </si>
+  <si>
+    <t>region</t>
+  </si>
+  <si>
+    <t>segmentoEdad</t>
+  </si>
+  <si>
+    <t>tienePareja</t>
+  </si>
+  <si>
+    <t>segmentoEducativo</t>
+  </si>
+  <si>
+    <t>horasHogar</t>
+  </si>
+  <si>
+    <t>ingresosTransferencias</t>
+  </si>
+  <si>
+    <t>ingresosOtros</t>
   </si>
 </sst>
 </file>
@@ -413,7 +464,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -467,82 +518,95 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -848,10 +912,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:J44"/>
+  <dimension ref="B2:K44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33:I33"/>
+      <selection activeCell="M28" sqref="M28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
@@ -865,9 +929,11 @@
     <col min="8" max="8" width="10.77734375" style="4" customWidth="1"/>
     <col min="9" max="9" width="18.33203125" style="3" customWidth="1"/>
     <col min="10" max="10" width="18.33203125" customWidth="1"/>
+    <col min="11" max="11" width="21.21875" customWidth="1"/>
+    <col min="12" max="12" width="11.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" s="3" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:11" s="3" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="12" t="s">
         <v>58</v>
       </c>
@@ -895,9 +961,12 @@
       <c r="J2" s="10" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B3" s="21" t="s">
+      <c r="K2" s="12" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="3" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B3" s="27" t="s">
         <v>59</v>
       </c>
       <c r="C3" s="7" t="s">
@@ -918,9 +987,10 @@
       </c>
       <c r="I3" s="20"/>
       <c r="J3" s="17"/>
-    </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B4" s="21"/>
+      <c r="K3" s="9"/>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B4" s="27"/>
       <c r="C4" s="7" t="s">
         <v>35</v>
       </c>
@@ -941,9 +1011,12 @@
         <v>4</v>
       </c>
       <c r="J4" s="17"/>
-    </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B5" s="21"/>
+      <c r="K4" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B5" s="27"/>
       <c r="C5" s="7" t="s">
         <v>37</v>
       </c>
@@ -964,9 +1037,12 @@
         <v>4</v>
       </c>
       <c r="J5" s="17"/>
-    </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B6" s="21"/>
+      <c r="K5" s="9" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B6" s="27"/>
       <c r="C6" s="7" t="s">
         <v>38</v>
       </c>
@@ -987,52 +1063,57 @@
         <v>4</v>
       </c>
       <c r="J6" s="17"/>
-    </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B7" s="21"/>
-      <c r="C7" s="39" t="s">
+      <c r="K6" s="9" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B7" s="27"/>
+      <c r="C7" s="48" t="s">
         <v>36</v>
       </c>
-      <c r="D7" s="35" t="s">
+      <c r="D7" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="36" t="s">
+      <c r="E7" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="37" t="s">
-        <v>4</v>
-      </c>
-      <c r="G7" s="38"/>
-      <c r="H7" s="37" t="s">
-        <v>4</v>
-      </c>
-      <c r="I7" s="38"/>
-      <c r="J7" s="17"/>
-    </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B8" s="29" t="s">
+      <c r="F7" s="51" t="s">
+        <v>4</v>
+      </c>
+      <c r="G7" s="21"/>
+      <c r="H7" s="51" t="s">
+        <v>4</v>
+      </c>
+      <c r="I7" s="21"/>
+      <c r="J7" s="51"/>
+      <c r="K7" s="50"/>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B8" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="C8" s="40"/>
-      <c r="D8" s="35" t="s">
+      <c r="C8" s="52"/>
+      <c r="D8" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="36" t="s">
+      <c r="E8" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="F8" s="37" t="s">
-        <v>4</v>
-      </c>
-      <c r="G8" s="38"/>
-      <c r="H8" s="37" t="s">
-        <v>4</v>
-      </c>
-      <c r="I8" s="38"/>
-      <c r="J8" s="17"/>
-    </row>
-    <row r="9" spans="2:10" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="B9" s="30"/>
-      <c r="C9" s="22" t="s">
+      <c r="F8" s="51" t="s">
+        <v>4</v>
+      </c>
+      <c r="G8" s="21"/>
+      <c r="H8" s="51" t="s">
+        <v>4</v>
+      </c>
+      <c r="I8" s="21"/>
+      <c r="J8" s="51"/>
+      <c r="K8" s="50"/>
+    </row>
+    <row r="9" spans="2:11" ht="30.15" x14ac:dyDescent="0.3">
+      <c r="B9" s="39"/>
+      <c r="C9" s="28" t="s">
         <v>34</v>
       </c>
       <c r="D9" s="13" t="s">
@@ -1052,10 +1133,13 @@
         <v>4</v>
       </c>
       <c r="J9" s="17"/>
-    </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B10" s="30"/>
-      <c r="C10" s="22"/>
+      <c r="K9" s="9" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B10" s="39"/>
+      <c r="C10" s="28"/>
       <c r="D10" s="13" t="s">
         <v>14</v>
       </c>
@@ -1073,10 +1157,13 @@
         <v>4</v>
       </c>
       <c r="J10" s="17"/>
-    </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B11" s="30"/>
-      <c r="C11" s="22"/>
+      <c r="K10" s="9" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B11" s="39"/>
+      <c r="C11" s="28"/>
       <c r="D11" s="13" t="s">
         <v>15</v>
       </c>
@@ -1094,10 +1181,13 @@
         <v>4</v>
       </c>
       <c r="J11" s="17"/>
-    </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B12" s="30"/>
-      <c r="C12" s="32" t="s">
+      <c r="K11" s="9" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B12" s="39"/>
+      <c r="C12" s="29" t="s">
         <v>73</v>
       </c>
       <c r="D12" s="13" t="s">
@@ -1113,14 +1203,17 @@
       <c r="H12" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="I12" s="26" t="s">
+      <c r="I12" s="35" t="s">
         <v>90</v>
       </c>
       <c r="J12" s="17"/>
-    </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B13" s="30"/>
-      <c r="C13" s="34"/>
+      <c r="K12" s="45" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B13" s="39"/>
+      <c r="C13" s="30"/>
       <c r="D13" s="13" t="s">
         <v>24</v>
       </c>
@@ -1134,12 +1227,13 @@
       <c r="H13" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="I13" s="27"/>
+      <c r="I13" s="36"/>
       <c r="J13" s="17"/>
-    </row>
-    <row r="14" spans="2:10" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="B14" s="30"/>
-      <c r="C14" s="34"/>
+      <c r="K13" s="46"/>
+    </row>
+    <row r="14" spans="2:11" ht="30.15" x14ac:dyDescent="0.3">
+      <c r="B14" s="39"/>
+      <c r="C14" s="30"/>
       <c r="D14" s="13" t="s">
         <v>26</v>
       </c>
@@ -1153,12 +1247,13 @@
       <c r="H14" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="I14" s="27"/>
+      <c r="I14" s="36"/>
       <c r="J14" s="17"/>
-    </row>
-    <row r="15" spans="2:10" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="B15" s="30"/>
-      <c r="C15" s="34"/>
+      <c r="K14" s="46"/>
+    </row>
+    <row r="15" spans="2:11" ht="30.15" x14ac:dyDescent="0.3">
+      <c r="B15" s="39"/>
+      <c r="C15" s="30"/>
       <c r="D15" s="13" t="s">
         <v>27</v>
       </c>
@@ -1172,12 +1267,13 @@
       <c r="H15" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="I15" s="27"/>
+      <c r="I15" s="36"/>
       <c r="J15" s="17"/>
-    </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B16" s="30"/>
-      <c r="C16" s="33"/>
+      <c r="K15" s="46"/>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B16" s="39"/>
+      <c r="C16" s="31"/>
       <c r="D16" s="13" t="s">
         <v>28</v>
       </c>
@@ -1191,32 +1287,38 @@
       <c r="H16" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="I16" s="28"/>
+      <c r="I16" s="37"/>
       <c r="J16" s="17"/>
-    </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B17" s="30"/>
+      <c r="K16" s="47"/>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B17" s="39"/>
       <c r="C17" s="41" t="s">
         <v>39</v>
       </c>
-      <c r="D17" s="35" t="s">
+      <c r="D17" s="42" t="s">
         <v>31</v>
       </c>
-      <c r="E17" s="36" t="s">
+      <c r="E17" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="F17" s="37" t="s">
-        <v>4</v>
-      </c>
-      <c r="G17" s="38"/>
-      <c r="H17" s="37" t="s">
-        <v>4</v>
-      </c>
-      <c r="I17" s="38"/>
+      <c r="F17" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="G17" s="20"/>
+      <c r="H17" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="I17" s="20" t="s">
+        <v>4</v>
+      </c>
       <c r="J17" s="17"/>
-    </row>
-    <row r="18" spans="2:10" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="B18" s="30"/>
+      <c r="K17" s="9" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11" ht="30.15" x14ac:dyDescent="0.3">
+      <c r="B18" s="39"/>
       <c r="C18" s="18" t="s">
         <v>42</v>
       </c>
@@ -1237,9 +1339,12 @@
         <v>4</v>
       </c>
       <c r="J18" s="17"/>
-    </row>
-    <row r="19" spans="2:10" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="B19" s="30"/>
+      <c r="K18" s="9" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="19" spans="2:11" ht="30.15" x14ac:dyDescent="0.3">
+      <c r="B19" s="39"/>
       <c r="C19" s="7" t="s">
         <v>45</v>
       </c>
@@ -1260,9 +1365,12 @@
         <v>4</v>
       </c>
       <c r="J19" s="17"/>
-    </row>
-    <row r="20" spans="2:10" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="B20" s="30"/>
+      <c r="K19" s="9" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="20" spans="2:11" ht="30.15" x14ac:dyDescent="0.3">
+      <c r="B20" s="39"/>
       <c r="C20" s="7" t="s">
         <v>46</v>
       </c>
@@ -1283,9 +1391,12 @@
         <v>4</v>
       </c>
       <c r="J20" s="17"/>
-    </row>
-    <row r="21" spans="2:10" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="B21" s="30"/>
+      <c r="K20" s="9" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="21" spans="2:11" ht="30.15" x14ac:dyDescent="0.3">
+      <c r="B21" s="39"/>
       <c r="C21" s="7" t="s">
         <v>51</v>
       </c>
@@ -1306,29 +1417,37 @@
         <v>4</v>
       </c>
       <c r="J21" s="17"/>
-    </row>
-    <row r="22" spans="2:10" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="B22" s="31"/>
-      <c r="C22" s="42" t="s">
+      <c r="K21" s="9" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="22" spans="2:11" ht="30.15" x14ac:dyDescent="0.3">
+      <c r="B22" s="40"/>
+      <c r="C22" s="44" t="s">
         <v>54</v>
       </c>
-      <c r="D22" s="35" t="s">
+      <c r="D22" s="42" t="s">
         <v>55</v>
       </c>
-      <c r="E22" s="36" t="s">
+      <c r="E22" s="43" t="s">
         <v>56</v>
       </c>
-      <c r="F22" s="37" t="s">
-        <v>4</v>
-      </c>
-      <c r="G22" s="38"/>
-      <c r="H22" s="37" t="s">
-        <v>4</v>
-      </c>
-      <c r="I22" s="38"/>
+      <c r="F22" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="G22" s="20"/>
+      <c r="H22" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="I22" s="20" t="s">
+        <v>4</v>
+      </c>
       <c r="J22" s="17"/>
-    </row>
-    <row r="23" spans="2:10" ht="30.15" x14ac:dyDescent="0.3">
+      <c r="K22" s="9" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="23" spans="2:11" ht="30.15" x14ac:dyDescent="0.3">
       <c r="B23" s="7" t="s">
         <v>71</v>
       </c>
@@ -1352,12 +1471,15 @@
         <v>4</v>
       </c>
       <c r="J23" s="17"/>
-    </row>
-    <row r="24" spans="2:10" ht="45.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="21" t="s">
+      <c r="K23" s="9" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="24" spans="2:11" ht="45.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="27" t="s">
         <v>72</v>
       </c>
-      <c r="C24" s="22" t="s">
+      <c r="C24" s="28" t="s">
         <v>74</v>
       </c>
       <c r="D24" s="8" t="s">
@@ -1375,14 +1497,17 @@
       <c r="H24" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="I24" s="23" t="s">
+      <c r="I24" s="32" t="s">
         <v>4</v>
       </c>
       <c r="J24" s="9"/>
-    </row>
-    <row r="25" spans="2:10" ht="15.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="21"/>
-      <c r="C25" s="22"/>
+      <c r="K24" s="45" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="25" spans="2:11" ht="15.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="27"/>
+      <c r="C25" s="28"/>
       <c r="D25" s="8" t="s">
         <v>61</v>
       </c>
@@ -1398,12 +1523,13 @@
       <c r="H25" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="I25" s="24"/>
+      <c r="I25" s="33"/>
       <c r="J25" s="17"/>
-    </row>
-    <row r="26" spans="2:10" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="B26" s="21"/>
-      <c r="C26" s="22"/>
+      <c r="K25" s="46"/>
+    </row>
+    <row r="26" spans="2:11" ht="30.15" x14ac:dyDescent="0.3">
+      <c r="B26" s="27"/>
+      <c r="C26" s="28"/>
       <c r="D26" s="8" t="s">
         <v>63</v>
       </c>
@@ -1419,12 +1545,13 @@
       <c r="H26" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="I26" s="24"/>
+      <c r="I26" s="33"/>
       <c r="J26" s="17"/>
-    </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B27" s="21"/>
-      <c r="C27" s="22"/>
+      <c r="K26" s="47"/>
+    </row>
+    <row r="27" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B27" s="27"/>
+      <c r="C27" s="28"/>
       <c r="D27" s="8" t="s">
         <v>64</v>
       </c>
@@ -1440,12 +1567,15 @@
       <c r="H27" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="I27" s="24"/>
+      <c r="I27" s="33"/>
       <c r="J27" s="17"/>
-    </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B28" s="21"/>
-      <c r="C28" s="22"/>
+      <c r="K27" s="45" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="28" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B28" s="27"/>
+      <c r="C28" s="28"/>
       <c r="D28" s="8" t="s">
         <v>65</v>
       </c>
@@ -1461,12 +1591,13 @@
       <c r="H28" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="I28" s="24"/>
+      <c r="I28" s="33"/>
       <c r="J28" s="17"/>
-    </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B29" s="21"/>
-      <c r="C29" s="22"/>
+      <c r="K28" s="46"/>
+    </row>
+    <row r="29" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B29" s="27"/>
+      <c r="C29" s="28"/>
       <c r="D29" s="8" t="s">
         <v>66</v>
       </c>
@@ -1482,12 +1613,13 @@
       <c r="H29" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="I29" s="24"/>
+      <c r="I29" s="33"/>
       <c r="J29" s="17"/>
-    </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B30" s="21"/>
-      <c r="C30" s="22"/>
+      <c r="K29" s="47"/>
+    </row>
+    <row r="30" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B30" s="27"/>
+      <c r="C30" s="28"/>
       <c r="D30" s="8" t="s">
         <v>85</v>
       </c>
@@ -1503,12 +1635,15 @@
       <c r="H30" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="I30" s="24"/>
+      <c r="I30" s="33"/>
       <c r="J30" s="9"/>
-    </row>
-    <row r="31" spans="2:10" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="B31" s="21"/>
-      <c r="C31" s="22"/>
+      <c r="K30" s="45" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="31" spans="2:11" ht="30.15" x14ac:dyDescent="0.3">
+      <c r="B31" s="27"/>
+      <c r="C31" s="28"/>
       <c r="D31" s="8" t="s">
         <v>86</v>
       </c>
@@ -1524,12 +1659,13 @@
       <c r="H31" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="I31" s="24"/>
+      <c r="I31" s="33"/>
       <c r="J31" s="9"/>
-    </row>
-    <row r="32" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B32" s="21"/>
-      <c r="C32" s="22"/>
+      <c r="K31" s="46"/>
+    </row>
+    <row r="32" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B32" s="27"/>
+      <c r="C32" s="28"/>
       <c r="D32" s="8" t="s">
         <v>88</v>
       </c>
@@ -1545,49 +1681,55 @@
       <c r="H32" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="I32" s="25"/>
+      <c r="I32" s="34"/>
       <c r="J32" s="9"/>
-    </row>
-    <row r="33" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="K32" s="47"/>
+    </row>
+    <row r="33" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B33" s="9"/>
-      <c r="C33" s="43" t="s">
+      <c r="C33" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="D33" s="44"/>
-      <c r="E33" s="45"/>
-      <c r="F33" s="46"/>
-      <c r="G33" s="47"/>
-      <c r="H33" s="46"/>
-      <c r="I33" s="47"/>
+      <c r="D33" s="23"/>
+      <c r="E33" s="24"/>
+      <c r="F33" s="25"/>
+      <c r="G33" s="26"/>
+      <c r="H33" s="25"/>
+      <c r="I33" s="26"/>
       <c r="J33" s="17"/>
-    </row>
-    <row r="34" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="K33" s="9"/>
+    </row>
+    <row r="34" spans="2:11" x14ac:dyDescent="0.3">
       <c r="C34"/>
     </row>
-    <row r="35" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:11" x14ac:dyDescent="0.3">
       <c r="C35"/>
     </row>
-    <row r="43" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:11" x14ac:dyDescent="0.3">
       <c r="E43" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="44" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:11" x14ac:dyDescent="0.3">
       <c r="E44" t="s">
         <v>79</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="13">
+    <mergeCell ref="I24:I32"/>
+    <mergeCell ref="I12:I16"/>
+    <mergeCell ref="B8:B22"/>
+    <mergeCell ref="K12:K16"/>
+    <mergeCell ref="K24:K26"/>
+    <mergeCell ref="K27:K29"/>
+    <mergeCell ref="K30:K32"/>
     <mergeCell ref="B3:B7"/>
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="C9:C11"/>
     <mergeCell ref="C12:C16"/>
     <mergeCell ref="B24:B32"/>
     <mergeCell ref="C24:C32"/>
-    <mergeCell ref="I24:I32"/>
-    <mergeCell ref="I12:I16"/>
-    <mergeCell ref="B8:B22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
code fixes and further prepared the database
</commit_message>
<xml_diff>
--- a/crosscheck.xlsx
+++ b/crosscheck.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="109">
   <si>
     <t>Variable</t>
   </si>
@@ -530,35 +530,56 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -571,27 +592,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -899,8 +899,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:K44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="K30" sqref="B24:K32"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
@@ -951,13 +951,13 @@
       </c>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B3" s="45" t="s">
+      <c r="B3" s="40" t="s">
         <v>59</v>
       </c>
-      <c r="C3" s="42" t="s">
+      <c r="C3" s="29" t="s">
         <v>57</v>
       </c>
-      <c r="D3" s="35" t="s">
+      <c r="D3" s="26" t="s">
         <v>2</v>
       </c>
       <c r="E3" s="24" t="s">
@@ -966,7 +966,9 @@
       <c r="F3" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="22"/>
+      <c r="G3" s="22" t="s">
+        <v>4</v>
+      </c>
       <c r="H3" s="25" t="s">
         <v>4</v>
       </c>
@@ -975,11 +977,11 @@
       <c r="K3" s="24"/>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B4" s="45"/>
-      <c r="C4" s="42" t="s">
+      <c r="B4" s="40"/>
+      <c r="C4" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="D4" s="35" t="s">
+      <c r="D4" s="26" t="s">
         <v>5</v>
       </c>
       <c r="E4" s="24" t="s">
@@ -988,7 +990,9 @@
       <c r="F4" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="22"/>
+      <c r="G4" s="22" t="s">
+        <v>4</v>
+      </c>
       <c r="H4" s="25" t="s">
         <v>4</v>
       </c>
@@ -1003,11 +1007,11 @@
       </c>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B5" s="45"/>
-      <c r="C5" s="42" t="s">
+      <c r="B5" s="40"/>
+      <c r="C5" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="D5" s="35" t="s">
+      <c r="D5" s="26" t="s">
         <v>7</v>
       </c>
       <c r="E5" s="24" t="s">
@@ -1016,7 +1020,9 @@
       <c r="F5" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="22"/>
+      <c r="G5" s="22" t="s">
+        <v>4</v>
+      </c>
       <c r="H5" s="25" t="s">
         <v>4</v>
       </c>
@@ -1031,11 +1037,11 @@
       </c>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B6" s="45"/>
-      <c r="C6" s="42" t="s">
+      <c r="B6" s="40"/>
+      <c r="C6" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="D6" s="35" t="s">
+      <c r="D6" s="26" t="s">
         <v>30</v>
       </c>
       <c r="E6" s="24" t="s">
@@ -1044,7 +1050,9 @@
       <c r="F6" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="G6" s="22"/>
+      <c r="G6" s="22" t="s">
+        <v>4</v>
+      </c>
       <c r="H6" s="25" t="s">
         <v>4</v>
       </c>
@@ -1059,8 +1067,8 @@
       </c>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B7" s="45"/>
-      <c r="C7" s="43" t="s">
+      <c r="B7" s="40"/>
+      <c r="C7" s="41" t="s">
         <v>36</v>
       </c>
       <c r="D7" s="19" t="s">
@@ -1072,7 +1080,9 @@
       <c r="F7" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="G7" s="22"/>
+      <c r="G7" s="22" t="s">
+        <v>4</v>
+      </c>
       <c r="H7" s="21" t="s">
         <v>4</v>
       </c>
@@ -1087,10 +1097,10 @@
       </c>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B8" s="27" t="s">
+      <c r="B8" s="33" t="s">
         <v>60</v>
       </c>
-      <c r="C8" s="44"/>
+      <c r="C8" s="42"/>
       <c r="D8" s="19" t="s">
         <v>11</v>
       </c>
@@ -1117,8 +1127,8 @@
       </c>
     </row>
     <row r="9" spans="2:11" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="B9" s="30"/>
-      <c r="C9" s="36" t="s">
+      <c r="B9" s="34"/>
+      <c r="C9" s="43" t="s">
         <v>34</v>
       </c>
       <c r="D9" s="23" t="s">
@@ -1147,8 +1157,8 @@
       </c>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B10" s="30"/>
-      <c r="C10" s="36"/>
+      <c r="B10" s="34"/>
+      <c r="C10" s="43"/>
       <c r="D10" s="23" t="s">
         <v>14</v>
       </c>
@@ -1175,8 +1185,8 @@
       </c>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B11" s="30"/>
-      <c r="C11" s="36"/>
+      <c r="B11" s="34"/>
+      <c r="C11" s="43"/>
       <c r="D11" s="23" t="s">
         <v>15</v>
       </c>
@@ -1203,8 +1213,8 @@
       </c>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B12" s="30"/>
-      <c r="C12" s="37" t="s">
+      <c r="B12" s="34"/>
+      <c r="C12" s="44" t="s">
         <v>73</v>
       </c>
       <c r="D12" s="23" t="s">
@@ -1222,19 +1232,19 @@
       <c r="H12" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="I12" s="26" t="s">
-        <v>4</v>
-      </c>
-      <c r="J12" s="27" t="s">
-        <v>4</v>
-      </c>
-      <c r="K12" s="28" t="s">
+      <c r="I12" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="J12" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="K12" s="36" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B13" s="30"/>
-      <c r="C13" s="38"/>
+      <c r="B13" s="34"/>
+      <c r="C13" s="45"/>
       <c r="D13" s="23" t="s">
         <v>24</v>
       </c>
@@ -1250,13 +1260,13 @@
       <c r="H13" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="I13" s="29"/>
-      <c r="J13" s="30"/>
-      <c r="K13" s="31"/>
+      <c r="I13" s="31"/>
+      <c r="J13" s="34"/>
+      <c r="K13" s="37"/>
     </row>
     <row r="14" spans="2:11" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="B14" s="30"/>
-      <c r="C14" s="38"/>
+      <c r="B14" s="34"/>
+      <c r="C14" s="45"/>
       <c r="D14" s="23" t="s">
         <v>26</v>
       </c>
@@ -1272,13 +1282,13 @@
       <c r="H14" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="I14" s="29"/>
-      <c r="J14" s="30"/>
-      <c r="K14" s="31"/>
+      <c r="I14" s="31"/>
+      <c r="J14" s="34"/>
+      <c r="K14" s="37"/>
     </row>
     <row r="15" spans="2:11" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="B15" s="30"/>
-      <c r="C15" s="38"/>
+      <c r="B15" s="34"/>
+      <c r="C15" s="45"/>
       <c r="D15" s="23" t="s">
         <v>27</v>
       </c>
@@ -1294,13 +1304,13 @@
       <c r="H15" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="I15" s="29"/>
-      <c r="J15" s="30"/>
-      <c r="K15" s="31"/>
+      <c r="I15" s="31"/>
+      <c r="J15" s="34"/>
+      <c r="K15" s="37"/>
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B16" s="30"/>
-      <c r="C16" s="39"/>
+      <c r="B16" s="34"/>
+      <c r="C16" s="46"/>
       <c r="D16" s="23" t="s">
         <v>28</v>
       </c>
@@ -1317,15 +1327,15 @@
         <v>4</v>
       </c>
       <c r="I16" s="32"/>
-      <c r="J16" s="33"/>
-      <c r="K16" s="34"/>
+      <c r="J16" s="35"/>
+      <c r="K16" s="38"/>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B17" s="30"/>
-      <c r="C17" s="40" t="s">
+      <c r="B17" s="34"/>
+      <c r="C17" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="D17" s="35" t="s">
+      <c r="D17" s="26" t="s">
         <v>31</v>
       </c>
       <c r="E17" s="24" t="s">
@@ -1351,11 +1361,11 @@
       </c>
     </row>
     <row r="18" spans="2:11" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="B18" s="30"/>
-      <c r="C18" s="41" t="s">
+      <c r="B18" s="34"/>
+      <c r="C18" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="D18" s="35" t="s">
+      <c r="D18" s="26" t="s">
         <v>43</v>
       </c>
       <c r="E18" s="24" t="s">
@@ -1381,11 +1391,11 @@
       </c>
     </row>
     <row r="19" spans="2:11" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="B19" s="30"/>
-      <c r="C19" s="42" t="s">
+      <c r="B19" s="34"/>
+      <c r="C19" s="29" t="s">
         <v>45</v>
       </c>
-      <c r="D19" s="35" t="s">
+      <c r="D19" s="26" t="s">
         <v>47</v>
       </c>
       <c r="E19" s="24" t="s">
@@ -1411,11 +1421,11 @@
       </c>
     </row>
     <row r="20" spans="2:11" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="B20" s="30"/>
-      <c r="C20" s="42" t="s">
+      <c r="B20" s="34"/>
+      <c r="C20" s="29" t="s">
         <v>46</v>
       </c>
-      <c r="D20" s="35" t="s">
+      <c r="D20" s="26" t="s">
         <v>50</v>
       </c>
       <c r="E20" s="24" t="s">
@@ -1441,11 +1451,11 @@
       </c>
     </row>
     <row r="21" spans="2:11" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="B21" s="30"/>
-      <c r="C21" s="42" t="s">
+      <c r="B21" s="34"/>
+      <c r="C21" s="29" t="s">
         <v>51</v>
       </c>
-      <c r="D21" s="35" t="s">
+      <c r="D21" s="26" t="s">
         <v>52</v>
       </c>
       <c r="E21" s="24" t="s">
@@ -1471,11 +1481,11 @@
       </c>
     </row>
     <row r="22" spans="2:11" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="B22" s="33"/>
-      <c r="C22" s="42" t="s">
+      <c r="B22" s="35"/>
+      <c r="C22" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="D22" s="35" t="s">
+      <c r="D22" s="26" t="s">
         <v>55</v>
       </c>
       <c r="E22" s="24" t="s">
@@ -1501,13 +1511,13 @@
       </c>
     </row>
     <row r="23" spans="2:11" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="B23" s="42" t="s">
+      <c r="B23" s="29" t="s">
         <v>71</v>
       </c>
-      <c r="C23" s="42" t="s">
+      <c r="C23" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="D23" s="35" t="s">
+      <c r="D23" s="26" t="s">
         <v>70</v>
       </c>
       <c r="E23" s="24" t="s">
@@ -1531,13 +1541,13 @@
       </c>
     </row>
     <row r="24" spans="2:11" ht="45.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="45" t="s">
+      <c r="B24" s="40" t="s">
         <v>72</v>
       </c>
-      <c r="C24" s="36" t="s">
+      <c r="C24" s="43" t="s">
         <v>74</v>
       </c>
-      <c r="D24" s="35" t="s">
+      <c r="D24" s="26" t="s">
         <v>82</v>
       </c>
       <c r="E24" s="24" t="s">
@@ -1552,20 +1562,20 @@
       <c r="H24" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="I24" s="46" t="s">
-        <v>4</v>
-      </c>
-      <c r="J24" s="45" t="s">
-        <v>4</v>
-      </c>
-      <c r="K24" s="28" t="s">
+      <c r="I24" s="39" t="s">
+        <v>4</v>
+      </c>
+      <c r="J24" s="40" t="s">
+        <v>4</v>
+      </c>
+      <c r="K24" s="36" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="25" spans="2:11" ht="15.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="45"/>
-      <c r="C25" s="36"/>
-      <c r="D25" s="35" t="s">
+      <c r="B25" s="40"/>
+      <c r="C25" s="43"/>
+      <c r="D25" s="26" t="s">
         <v>61</v>
       </c>
       <c r="E25" s="24" t="s">
@@ -1580,14 +1590,14 @@
       <c r="H25" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="I25" s="46"/>
-      <c r="J25" s="45"/>
-      <c r="K25" s="31"/>
+      <c r="I25" s="39"/>
+      <c r="J25" s="40"/>
+      <c r="K25" s="37"/>
     </row>
     <row r="26" spans="2:11" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="B26" s="45"/>
-      <c r="C26" s="36"/>
-      <c r="D26" s="35" t="s">
+      <c r="B26" s="40"/>
+      <c r="C26" s="43"/>
+      <c r="D26" s="26" t="s">
         <v>63</v>
       </c>
       <c r="E26" s="24" t="s">
@@ -1602,14 +1612,14 @@
       <c r="H26" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="I26" s="46"/>
-      <c r="J26" s="45"/>
-      <c r="K26" s="34"/>
+      <c r="I26" s="39"/>
+      <c r="J26" s="40"/>
+      <c r="K26" s="38"/>
     </row>
     <row r="27" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B27" s="45"/>
-      <c r="C27" s="36"/>
-      <c r="D27" s="35" t="s">
+      <c r="B27" s="40"/>
+      <c r="C27" s="43"/>
+      <c r="D27" s="26" t="s">
         <v>64</v>
       </c>
       <c r="E27" s="24" t="s">
@@ -1624,20 +1634,20 @@
       <c r="H27" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="I27" s="46" t="s">
-        <v>4</v>
-      </c>
-      <c r="J27" s="45" t="s">
-        <v>4</v>
-      </c>
-      <c r="K27" s="28" t="s">
+      <c r="I27" s="39" t="s">
+        <v>4</v>
+      </c>
+      <c r="J27" s="40" t="s">
+        <v>4</v>
+      </c>
+      <c r="K27" s="36" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="28" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B28" s="45"/>
-      <c r="C28" s="36"/>
-      <c r="D28" s="35" t="s">
+      <c r="B28" s="40"/>
+      <c r="C28" s="43"/>
+      <c r="D28" s="26" t="s">
         <v>65</v>
       </c>
       <c r="E28" s="24" t="s">
@@ -1652,14 +1662,14 @@
       <c r="H28" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="I28" s="46"/>
-      <c r="J28" s="45"/>
-      <c r="K28" s="31"/>
+      <c r="I28" s="39"/>
+      <c r="J28" s="40"/>
+      <c r="K28" s="37"/>
     </row>
     <row r="29" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B29" s="45"/>
-      <c r="C29" s="36"/>
-      <c r="D29" s="35" t="s">
+      <c r="B29" s="40"/>
+      <c r="C29" s="43"/>
+      <c r="D29" s="26" t="s">
         <v>66</v>
       </c>
       <c r="E29" s="24" t="s">
@@ -1674,14 +1684,14 @@
       <c r="H29" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="I29" s="46"/>
-      <c r="J29" s="45"/>
-      <c r="K29" s="34"/>
+      <c r="I29" s="39"/>
+      <c r="J29" s="40"/>
+      <c r="K29" s="38"/>
     </row>
     <row r="30" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B30" s="45"/>
-      <c r="C30" s="36"/>
-      <c r="D30" s="35" t="s">
+      <c r="B30" s="40"/>
+      <c r="C30" s="43"/>
+      <c r="D30" s="26" t="s">
         <v>85</v>
       </c>
       <c r="E30" s="24" t="s">
@@ -1696,20 +1706,20 @@
       <c r="H30" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="I30" s="46" t="s">
-        <v>4</v>
-      </c>
-      <c r="J30" s="45" t="s">
-        <v>4</v>
-      </c>
-      <c r="K30" s="28" t="s">
+      <c r="I30" s="39" t="s">
+        <v>4</v>
+      </c>
+      <c r="J30" s="40" t="s">
+        <v>4</v>
+      </c>
+      <c r="K30" s="36" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="31" spans="2:11" ht="30.15" x14ac:dyDescent="0.3">
-      <c r="B31" s="45"/>
-      <c r="C31" s="36"/>
-      <c r="D31" s="35" t="s">
+      <c r="B31" s="40"/>
+      <c r="C31" s="43"/>
+      <c r="D31" s="26" t="s">
         <v>86</v>
       </c>
       <c r="E31" s="24" t="s">
@@ -1724,14 +1734,14 @@
       <c r="H31" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="I31" s="46"/>
-      <c r="J31" s="45"/>
-      <c r="K31" s="31"/>
+      <c r="I31" s="39"/>
+      <c r="J31" s="40"/>
+      <c r="K31" s="37"/>
     </row>
     <row r="32" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B32" s="45"/>
-      <c r="C32" s="36"/>
-      <c r="D32" s="35" t="s">
+      <c r="B32" s="40"/>
+      <c r="C32" s="43"/>
+      <c r="D32" s="26" t="s">
         <v>88</v>
       </c>
       <c r="E32" s="24" t="s">
@@ -1746,9 +1756,9 @@
       <c r="H32" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="I32" s="46"/>
-      <c r="J32" s="45"/>
-      <c r="K32" s="34"/>
+      <c r="I32" s="39"/>
+      <c r="J32" s="40"/>
+      <c r="K32" s="38"/>
     </row>
     <row r="33" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B33" s="7"/>
@@ -1782,11 +1792,12 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="I12:I16"/>
-    <mergeCell ref="B8:B22"/>
-    <mergeCell ref="K12:K16"/>
-    <mergeCell ref="K24:K26"/>
-    <mergeCell ref="K27:K29"/>
+    <mergeCell ref="B3:B7"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="C12:C16"/>
+    <mergeCell ref="B24:B32"/>
+    <mergeCell ref="C24:C32"/>
     <mergeCell ref="K30:K32"/>
     <mergeCell ref="J12:J16"/>
     <mergeCell ref="I24:I26"/>
@@ -1795,12 +1806,11 @@
     <mergeCell ref="J24:J26"/>
     <mergeCell ref="J27:J29"/>
     <mergeCell ref="J30:J32"/>
-    <mergeCell ref="B3:B7"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="C9:C11"/>
-    <mergeCell ref="C12:C16"/>
-    <mergeCell ref="B24:B32"/>
-    <mergeCell ref="C24:C32"/>
+    <mergeCell ref="I12:I16"/>
+    <mergeCell ref="B8:B22"/>
+    <mergeCell ref="K12:K16"/>
+    <mergeCell ref="K24:K26"/>
+    <mergeCell ref="K27:K29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>